<commit_message>
- updated data source content in excel
</commit_message>
<xml_diff>
--- a/InfluencePWA/Data/Source/influenceDataExcel.xlsx
+++ b/InfluencePWA/Data/Source/influenceDataExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hustler Joon\source\repos\InfluencePWA\InfluencePWA\Data\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9B97F3-392D-42D8-BBE7-1B7E2257E4B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CD1450-01B1-4545-9FA2-620D900E0AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E2376BE-168A-49C5-9AFA-A2935957CF1D}"/>
+    <workbookView xWindow="-28920" yWindow="-3705" windowWidth="29040" windowHeight="15840" xr2:uid="{3E2376BE-168A-49C5-9AFA-A2935957CF1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,13 +82,6 @@
     <t>Natural Powers</t>
   </si>
   <si>
-    <t>Build into the creative process an initial period that is open-ended.
-Have wide knowledge of multiple fields.
-Never settle into complacency, as if your initial vision represents the endpoint.
-Finally, you must come to embrace slowness as a virtue in itself.
-Imagine yourself years in the future looking back at the work you have done. From that future vantage point, the extra months and years you devoted to the process will not seem painful or laborious at all.</t>
-  </si>
-  <si>
     <t>The Open Field</t>
   </si>
   <si>
@@ -123,12 +116,6 @@
     <t>Strategies for Acquiring Social Intelligence</t>
   </si>
   <si>
-    <t>Speak through your work - be efficient, detail-oriented, and make what you write or present clear and easy to follow, and this will show your care for the audience or public at large.
-Craft the appropriate persona - people will judge you based on your outward appearance - be aware of this and plan for it.
-See yourself as others see you - look at negative events in your past and dissect these occurrences.  What patterns can we observe that reveal flaws in our character?  Seek opinions from those you trust about your behaviour as well, and begin to cultivate the ability to see yourself as you really are.
-Suffer fools gladly - they are simply part of life, like rocks or furniture.  Smile at their antics, tolerate their presence, and avoid the madness of trying to change them.</t>
-  </si>
-  <si>
     <t>Strategies for Completing the Ideal Apprenticeship</t>
   </si>
   <si>
@@ -220,15 +207,6 @@
   </si>
   <si>
     <t>Synthesize all forms of knowledge: The Universal Man/Woman</t>
-  </si>
-  <si>
-    <t>Oddly enough, they discovered that what really makes successful entrepreneurs is not the nature of their idea, or the university they went to, but their actual character: their willingness to adapt their idea and take advantage of possibilities they had not first imagined. This is precisely the trait: fluidity of mind: that Graham had identified in himself and in other inventors. The other essential character trait was supreme tenacity.
-The lesson is simple: what constitutes true creativity is the openness and adaptability of our spirit. When we see or experience something we must be able to look at it from several angles, to see other possibilities beyond the obvious ones.
-The difference then is not in some initial creative power of the brain, but in how we look at the world and the fluidity with which we can reframe what we see. Creativity and adaptability are inseparable.</t>
-  </si>
-  <si>
-    <t>If You Must Find Fault, This Is the Way to Begin. 
-What has someone done well? Where can you agree? What is working? Carnegie encourages readers to start all interactions :  especially ones that have the potential for disagreement, with honest appreciation.</t>
   </si>
   <si>
     <t>There are many paths to mastery, and if you are persistent you will certainly find one that suits you. But a key component in the process is determining your mental and psychological strengths and working with them. To rise to the level of mastery requires many hours of dedicated focus and practice. You cannot get there if your work brings you no joy and you are constantly struggling to overcome your own weaknesses. You must look deep within and come to an understanding of these particular strengths and weaknesses you possess, being as realistic as possible. Once you start in this direction, you will gain momentum. You will not be burdened by conventions, and you will not be slowed down by having to deal with skills that go against your inclinations and strengths. In this way, your creative and intuitive powers will be naturally awakened.
@@ -269,13 +247,6 @@
 If you have feedback for someone or want to challenge someone's opinion, you want to do it privately. Nothing is more shameful than being reprimanded or corrected in front of a large group of people. Think about someone's ego if you do have to give them a Poop Sandwich. Do it privately and maybe at the end of a day or before a weekend so they can head home to process in private.</t>
   </si>
   <si>
-    <t>How to Spur Men on to Success. 
-While Carnegie encourages readers to be careful and hold back criticism or judgment, he says to lavish genuine praise whenever it is warranted. Here are some ideas:
-Thank people for their work.
-Compliment any exceptional traits or qualities.
-Be specific with your compliments :  and don't give everyone the same compliments!</t>
-  </si>
-  <si>
     <t>Promise to think over your opponent's ideas and study them carefully</t>
   </si>
   <si>
@@ -357,12 +328,6 @@
   </si>
   <si>
     <t>Mastery</t>
-  </si>
-  <si>
-    <t>Friends</t>
-  </si>
-  <si>
-    <t>Human</t>
   </si>
   <si>
     <t>Don't criticize, condemn or complain</t>
@@ -408,40 +373,22 @@
     <t>Get others to do the work for you, but always take the credit</t>
   </si>
   <si>
-    <t>Use the wisdom, knowledge, and legwork of other people to further your own cause.  Not only will such assistance save you valuable time and energy, it will give you a godlike aura of efficiency and speed.  In the end, your helpers will be forgotten and you will be remembered. Never do yourself what others can do for you.</t>
-  </si>
-  <si>
     <t>Win through your actions, never through argument</t>
   </si>
   <si>
-    <t>Any momentary triumph you think gained through argument is really a Pyrrhic victory:  The resentment and ill will you stir up is stronger and lasts longer than any momentary change of opinion.  It is much more powerful to get others to agree with you through your actions, without saying a word. Demonstrate, do not explicate.</t>
-  </si>
-  <si>
     <t>Infection: Avoid the unhappy or the unlucky</t>
   </si>
   <si>
     <t>Learn to keep people dependent on you</t>
   </si>
   <si>
-    <t>To maintain your independence you must always be needed and wanted.  The more you are relied on, the more freedom you have. Make people depend on you for their happiness and prosperity and you have nothing to fear.  Never teach them enough so that they can do without you.</t>
-  </si>
-  <si>
     <t>Use selective honesty and generosity to disarm your victim</t>
   </si>
   <si>
-    <t>If you need to turn to an ally for help, do not bother to remind him of your past assistance and good deeds.  He will find a way to ignore you. Instead, uncover something in your request, or in your alliance with him, that will benefit him, and emphasize it out of all proportion.  He will respond enthusiastically when he sees something to be gained for himself.</t>
-  </si>
-  <si>
     <t>Pose as a friend, work as a spy</t>
   </si>
   <si>
-    <t>Knowing about your rival is critical.  Use spies to gather valuable information that will keep you a step ahead.  Better still: Play the spy yourself. In polite social encounters, learn to probe.  Ask indirect questions to get people to reveal their weaknesses and intentions. There is no occasion that is not an opportunity for artful spying.</t>
-  </si>
-  <si>
     <t>Crush your enemy totally</t>
-  </si>
-  <si>
-    <t>All great leaders since Moses have known that a feared enemy must be crushed completely.  (Sometimes they have learned this the hard way.) If one ember is left alight, no matter how dimly it smolders, a fire will eventually break out.  More is lost through stopping halfway than through total annihilation: The enemy will recover and will seek revenge. Crush him, not only in body but in spirit.</t>
   </si>
   <si>
     <t>Use absence to increase respect and hono</t>
@@ -474,51 +421,27 @@
     <t>Play the perfect courtier</t>
   </si>
   <si>
-    <t xml:space="preserve">The perfect courtier thrives in a world where everything revolves around power and political dexterity.  He has mastered the art of indirection; he flatters, yields to superiors, and asserts power over others in the most oblique and graceful manner.  Learn and apply the laws of courtiership and there will be no limit to how far you can rise in the court. </t>
-  </si>
-  <si>
     <t>Re-create yourself</t>
   </si>
   <si>
     <t>Keep your hands clean</t>
   </si>
   <si>
-    <t>People have an overwhelming desire to believe in something.  Become the focal point of such desire by offering them a cause, a new faith to follow.  Keep your words vague but full of promise; emphasize enthusiasm over rationality and clear thinking. Give your new disciples rituals to perform, ask them to make sacrifices on your behalf.  In the absence of organized religion and grand causes, your new belief system will bring you untold power.</t>
-  </si>
-  <si>
     <t>Enter action with boldness</t>
   </si>
   <si>
-    <t>Lions circle the hesitant prey.
-Boldness strikes fear, fear creates authority.
-Going halfway with half a heart digs a deeper grave.
-Hesitation creates gaps, boldness obliterates them.
-Audacity separates you from the herd.
-When you are as small and obscure as David was, you must find a Goliath to attack. The larger the target, the more attention you gain.
-Timidity is dangerous:  Better to enter with boldness. Any mistakes you commit through audacity are easily corrected with more audacity. Everyone admires the bold; no one honors the timid.</t>
-  </si>
-  <si>
     <t>Plan all the way to the end</t>
   </si>
   <si>
-    <t>The ending is everything.  Plan all the way to it, taking into account all the possible consequences, obstacles, and twists of fortune that might reverse your hard work and give the glory to others.  By planning to the end you will not be overwhelmed by circumstances and you will know when to stop. Gently guide fortune and help determine the future by thinking far ahead.</t>
-  </si>
-  <si>
     <t>Make your accomplishments seem effortless</t>
   </si>
   <si>
     <t>Control the options: get others to play with the cards you deal</t>
   </si>
   <si>
-    <t>Everyone has a weakness, a gap in the castle wall.  That weakness is usually an insecurity, an uncontrollable emotion or need; it can also be a small secret pleasure.  Either way, once found it is a thumbscrew you can turn to your advantage.</t>
-  </si>
-  <si>
     <t>Be royal in your own fashion: act like a king to be treated like one</t>
   </si>
   <si>
-    <t>The way you carry yourself will often determine how you are treated; In the long run, appearing vulgar or common will make people disrespect you.  For a king respects himself and inspires the same sentiment in others. By acting regally and confident of your powers, you make yourself seem destined to wear a crown.</t>
-  </si>
-  <si>
     <t>Master the art of timing</t>
   </si>
   <si>
@@ -531,62 +454,31 @@
     <t>Think as you like but behave like others</t>
   </si>
   <si>
-    <t>If you make a show of going against the times, flaunting your unconventional ideas and unorthodox ways, people will think that you only want attention and that you look down upon them.  They will find a way to punish you for making them feel inferior. It is far safer to blend in and nurture the common touch. Share your originality only with tolerant friends and those who are sure to appreciate your uniqueness.</t>
-  </si>
-  <si>
     <t>Stir up waters to catch fish</t>
   </si>
   <si>
-    <t>Anger and emotion are strategically counterproductive.  You must always stay calm and objective. But if you can make your enemies angry while staying calm yourself, you gain a decided advantage.  Put your enemies off-balance: Find the chink in their vanity through which you can rattle them and you hold the strings.</t>
-  </si>
-  <si>
     <t>Despise the free lunch</t>
   </si>
   <si>
-    <t>What happens first always appears better and more original than what comes after.  If you succeed a great man or have a famous parent, you will have to accomplish double their achievements to outshine them.  Do not get lost in their shadow, or stuck in a past, not of your own making: Establish your own name and identity by changing course.  Slay the overbearing father, disparage his legacy, and gain power by shining in your own way.</t>
-  </si>
-  <si>
     <t>Strike the shepherd and the sheep will scatter</t>
   </si>
   <si>
     <t>Work on the hearts and minds of others</t>
   </si>
   <si>
-    <t>Coercion creates a reaction that will eventually work against you.  You must seduce others into wanting to move in your direction. A person you have seduced becomes your loyal pawn.  And the way to seduce others is to operate on their individual psychologies and weaknesses. Soften up the resistant by working on their emotions, playing on what they hold dear and what they fear.  Ignore the hearts and minds of others and they will grow to hate you.</t>
-  </si>
-  <si>
     <t>Disarm and infuriate with the mirror effect</t>
   </si>
   <si>
-    <t>The mirror reflects reality, but it is also the perfect tool for deception: When you mirror your enemies, doing exactly as they do, they cannot figure out your strategy.  The Mirror Effect mocks and humiliates them, making them overreact. By holding up a mirror to their psyches, you seduce them with the illusion that you share their values; by holding up a mirror to their actions, you teach them a lesson.  Few can resist the power of the Mirror Effect.</t>
-  </si>
-  <si>
     <t>Preach the need for change, but never reform too much at once</t>
   </si>
   <si>
-    <t>Everyone understands the need for change in the abstract, but on the day-to-day level, people are creatures of habit.  Too much innovation is traumatic and will lead to revolt. If you are new to a position of power, or an outsider trying to build a power base, make a show of respecting the old way of doing things.  If change is necessary, make it feel like a gentle improvement on the past.</t>
-  </si>
-  <si>
     <t>Never appear too perfect</t>
   </si>
   <si>
-    <t>Appearing better than others is always dangerous, but most dangerous of all is to appear to have no faults or weaknesses.  Envy creates silent enemies. It is smart to occasionally display defects, and admit to harmless vices, in order to deflect envy and appear more human and approachable.  Only gods and the dead can seem perfect with impunity.
-Do not try to help or do favors for those who envy you; they will think you are condescending to them.</t>
-  </si>
-  <si>
     <t>Do not go past the mark you aimed for; in victory, learn when to stop</t>
   </si>
   <si>
-    <t>The moment of victory is often the moment of greatest peril.  In the heat of victory, arrogance and overconfidence can push you past the goal you had aimed for, and by going too far, you make more enemies than you defeat.  Do not allow success to go to your head. There is no substitute for strategy and careful planning. Set a goal, and when you reach it, stop.</t>
-  </si>
-  <si>
     <t>Assume formlessness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">By taking a shape, by having a visible plan, you open yourself to attack.  Instead of taking a form for your enemy to grasp, keep yourself adaptable and on the move.  Accept the fact that nothing is certain and no law is fixed. The best way to protect yourself is to be as fluid and formless as water; never bet on stability or lasting order.  Everything changes.  </t>
-  </si>
-  <si>
-    <t>Power</t>
   </si>
   <si>
     <t>Declare war on your enemies: Polarity Strategy</t>
@@ -652,13 +544,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Defeat them in detail: Divide and Conquer</t>
-  </si>
-  <si>
-    <t>Sow the seeds of discontent, turn a large enemies into smaller parts. Then attack and conquer.
-Romans divided the power base of their captured areas so that no one area had the power to attack.
-Divide groups and they are easier to conquer.
-Historically people have banded together to defend themselves, deny them this comfort.
-Surprise and splinter the group attacking the pieces.</t>
   </si>
   <si>
     <t>The flank attack: Turning</t>
@@ -719,27 +604,10 @@
     <t>Destroy from within: The Inner Front</t>
   </si>
   <si>
-    <t>Instead of fighting your enemies: join them.
-Infiltrate their ranks, rise to the top. Then slowly get what you want or stage a coup.Do not attack the walls of the fort, attack from within.
-Exploit the disaffected with your opponent and use them.
-Undermine the morale of your opponent's troops.
-Befriend your opponent and work from within their mind.
-Be patient and take small steps.
-Keep your group of conspirators small.</t>
-  </si>
-  <si>
     <t>Seeming to submit to dominate: Passive-Aggression</t>
   </si>
   <si>
     <t>Sow panic with terror: Chain Reaction</t>
-  </si>
-  <si>
-    <t>War</t>
-  </si>
-  <si>
-    <t>Law: All of us have masculine and feminine qualities. But in the need to present a consistent identity in society, we tend to repress these qualities, overidentifying with the masculine or feminine role expected of us. Thereby we lose valuable dimensions to our character.
-Example: Caterina Sforza became an Italian noblewoman and Countess of ForlÃ¬ and Lady of Imola. Such titles were unusual for women in her time. In the author's opinion her masculine qualities helped her to achieve this.
-Advice: You must become aware of these lost masculine or feminine traits and slowly reconnect to them, unleashing creative powers in the process.</t>
   </si>
   <si>
     <t>When asking for help, appeal to people's self-interest, never to their mercy or gratitude</t>
@@ -749,13 +617,6 @@
 At the start of an affair, you need to heighten your presence in the eyes of the other. If you absent yourself too early, you may be forgotten. But once your lover's emotions are engaged, and the feeling of love has crystallized, absence inflames and excites. Giving no reason for your absence excites even more.</t>
   </si>
   <si>
-    <t>Humans are creatures of habit with an insatiable need to see familiarity in other people's actions.  Your predictability gives them a sense of control. Turn the tables: Be deliberately unpredictable. Behavior that seems to have no consistency or purpose will keep them off-balance, and they will wear themselves out trying to explain your moves.  Taken to an extreme, this strategy can intimidate and terrorize.
-Too much unpredictability will be seen as a sign of indecisiveness, or even of some more serious psychic problem. Patterns are powerful, and you can terrify people by disrupting them. Such power should only be used judiciously.</t>
-  </si>
-  <si>
-    <t>You must seem a paragon of civility and efficiency: Your hands are never soiled by mistakes and nasty deeds.  Maintain such a spotless appearance by using others as scapegoats and cat's-paws to disguise your involvement.</t>
-  </si>
-  <si>
     <t>Play on people's need to create a cult like following</t>
   </si>
   <si>
@@ -766,17 +627,6 @@
   </si>
   <si>
     <t>Avoid stepping into a great man's shoes</t>
-  </si>
-  <si>
-    <t>Do not become a sheep in the crowded center: go to the extreme. A dominating polarizing presence has more pull than middle ground men.
-Don't necessarily get into the idea you need to be liked -as in How to Win Friends-, being respected is better, and even being feared. Don't be afraid of battles and enemies either. Your enemies give you a purpose and direction.
-And battles are what will allow you to win.
-And ultimately, it's victory over your enemies will bring you the most meaningful and lasting popularity.
-Victory over your enemies is the best form of popularity
-Reversal:
-Don't see enemies everywhere, and always keep it for yourself. If you're wrong, nobody will judge you.
-Do like Cortez did. Keep it to yourself, pretend you didn't notice. Let them come more and more on the surface, and when it's obvious to everyone they're enemies, then strike.
-And don't make enemies and pick fights at any time. You don't want to make enemies of everyone.</t>
   </si>
   <si>
     <t>Detach yourself from the fog of war and chaos of battles.
@@ -787,20 +637,6 @@
 Greene says that we tend to overestimate others and trust ourselves less. Overcompansate it by doing it the opposite: trust yourself more and trust others less.</t>
   </si>
   <si>
-    <t>People naturally have their own agendas in the groups you lead.
-If you're too authoritarian they will resent you, and if you're too lax they will revert doing their own interests.
-You need a chain of command where people buy into your vision and follow your lead naturally.
-The overall strategic vision must come from you and you alone. But make the group feel involved in the decision making. Take their good ideas, deflect the bad ones and if necessary make minor changes to appease the most political ones.
-The Dangers of Groupthink
-People in group tend to act and speak conservatively as they're all worried of what others think.
-That's not what you need. And that's why you need unity of command (you).
-Beware of Political Animals
-Political animals not only are after themselves, but form factions to further their agendas and create their small fiefdoms of power.
-You should avoid hiring these people in the first place.
-Watch out for those who mirror your ideas 1:1, they're probably trying to ingratiate you.
-If it's too late, isolate them</t>
-  </si>
-  <si>
     <t>People are cynical nowadays, speeches and group activities do little.
 Build a group myth. Use the past to forge an idea that your group is mythical and legendary. People will feel the pride and work hard to live up to that image.
 Those who don't want to will be forced by the shaming pressure of their own peers.
@@ -816,11 +652,6 @@
 Once you're engaged make sure you don't lose because you're cutting costs. That's not economy but stupidity.</t>
   </si>
   <si>
-    <t>Let them go first. Let them believe you're weak.
-Than destroy them with a counterattack once they're over-stretched.
-The best blows are the ones they never see coming</t>
-  </si>
-  <si>
     <t>Make your enemy believe you're too difficult to attack.
 Look stronger than they think, build a reputation for fighting till the bitter end, sometimes taking your enemy with you. This works great with enemies who have a reputation.
 If you're smaller, they have little to gain and much to lose.
@@ -870,15 +701,6 @@
 Before the battle begins, put your opponent in a position of such weakness that victory is easy and quick. Create dilemmas where all potential choices are bad.</t>
   </si>
   <si>
-    <t>Don't trust people's words.
-They will break their promises and find moral justifications for their amoral behaviors.
-And people will forget broken promises when you're strong and in the position to offer something they want.
-Keep advancing and waging wars during negotiations.
-When you keep winning the war you will get better deals and you can use the conquered terrain as bargaining chips. If on the other hand you stop, you will often find your enemy much stronger in battle because he didn't stop.
-It's even more important you keep advancing when you're holding the week hand, so you can show resolve.
-Act strong and people will treat you as strong.</t>
-  </si>
-  <si>
     <t>Deception is not about making big shows of elaborate distractions.
 Most people are aware you'll try to deceive them and won't fall for it. The best deceptions mix reality with fiction.
 Spread your deceptions to people who believe in the lie themselves, and they'll work to convince others, naturally, of your deception.
@@ -893,18 +715,6 @@
     <t>Make your cause seem morally justified and paint your enemy as evil.
 Pick a fight with an enemy you can portray as morally corrupt, authoritarian, or power hungry. Don't drum up your moral superiority but show it: contrast your own life with theirs.
 Convince people you're fighting for a just moral cause and nobody will take note of the tactics you deploy.</t>
-  </si>
-  <si>
-    <t>Most people operate with feelings and emotions and make alliances based on liking and friendships.
-Bad strategy: the best alliances are the ones giving something you can't get on your own.
-Sometimes we think instead that the more allies the better. But it's not true: the more you have, the more likely it is you'll be dragged into other people's wars.
-Alliances must be based on mutual interests. See them as stepping stones towards getting what you need.
-Finally, never become too dependent on alliances: they will drop you when it best serves them.
-Alliances Strategies:
-Seem like you want to help and let them do the work, then reap the benefits.
-You'll be accused of playing the alliance game, which are nothing but strategic moral attacks. The only real danger is that your reputation will be so tarnished that people won't wanna ally to you anymore.
-But, says Greene:
-Self interest rules the world</t>
   </si>
   <si>
     <t>Sometimes enemies are your colleagues, your collaborators.
@@ -913,10 +723,6 @@
 Get under their skin subtly instead. It works best with people who need to perform as they won't be able to be at their best.
 Instill doubts and insecurities in rivals, getting them to think too much and act defensively. Make them hang themselves through their own self-destructive tendencies, leaving you blameless and clean.
 Rigid types who cannot stand breaking moral codes are the easiest to one-up. They will overreact and attack you too obviously, making them look vindictive.</t>
-  </si>
-  <si>
-    <t>Most people cling to status quo and are loath of starting wars over trivial matters.
-That's why you will take small bites, bite by bite. Every time it will be too small to start a war and once you take enough bites they won't even be able to wage war against you.</t>
   </si>
   <si>
     <t>The goal of communication is to further your interest, to penetrate the enemies' minds. Anything else is self indulgent talk.
@@ -935,64 +741,19 @@
 If it's a partner in a relationship, make them feel safe to express themselves.</t>
   </si>
   <si>
-    <t>Terror strategies aim at raising havoc, making enemies fearful and provoking desperate overreactions -or surrenders without fighting-.
-They serve well to smaller groups who can't fight openly because of size disparity.
-Their goal is to spread fear with small acts of violence that reverberate through stories and media and command outsized attention compared to their real effect.</t>
-  </si>
-  <si>
     <t>Make the other person feel important - and do it sincerely</t>
   </si>
   <si>
     <t>Make other people come to you - use bait if necessary</t>
   </si>
   <si>
-    <t>For negotiations or meetings, it is always wise to lure others into your territory, or the territory of your choice. You have your bearings, while they see nothing familiar and are subtly placed on the defensive.
-When you force the other person to act, you are the one in control.  It is always better to make your opponent come to you, abandoning his own plans in the process.  Lure him with fabulous gains - then attack. You hold the cards.</t>
-  </si>
-  <si>
-    <t>You can die from someone else's misery - emotional states are as infectious as disease.  You may feel you are helping the drowning man but you are only precipitating your own disaster.  The unfortunate sometimes draw misfortune on themselves; they will also draw it on you. Associate with the happy and fortunate instead.
-When you suspect you are in the presence of an infector, don't argue, don't try to help, don't pass the person on to your friends, or you will become enmeshed. Flee the infector's presence or suffer the consequences.</t>
-  </si>
-  <si>
-    <t>One sincere and honest move will cover over dozens of dishonest ones.  Open-hearted gestures of honesty and generosity bring down the guard of even the most suspicious people.  Once your selective honesty opens a hole in their armor, you can deceive and manipulate them at will. A timely gift - a Trojan horse - will serve the same purpose.</t>
-  </si>
-  <si>
     <t>Do not build fortresses to protect yourself - isolation is dangerous</t>
   </si>
   <si>
-    <t>The world is dangerous and enemies are everywhere - everyone has to protect themselves.  A fortress seems the safest. But isolation exposes you to more dangers than it protects you from - it cuts you off from valuable information, it makes you conspicuous and an easy target.  Better to circulate among people, find allies, mingle. You are shielded from your enemies by the crowd.</t>
-  </si>
-  <si>
     <t>Know who you're dealing with - do not offend the wrong person</t>
   </si>
   <si>
-    <t>There are many different kinds of people in the world, and you can never assume that everyone will react to your strategies in the same way.  Deceive or outmaneuver some people and they will spend the rest of their lives seeking revenge. They are wolves in lambs' clothing. Choose your victims and opponents carefully, then - never offend or deceive the wrong person.</t>
-  </si>
-  <si>
     <t>Play a sucker to catch a sucker - seem dumber than your mark</t>
-  </si>
-  <si>
-    <t>Given how important the idea of intelligence is to most people's vanity, it is critical never inadvertently to insult or impugn a person's brain power.
-No one likes feeling stupider than the next person.  The trick, then, is to make your victims feel smart - and not just smart, but smarter than you are.  Once convinced of this, they will never suspect that you may have ulterior motives.</t>
-  </si>
-  <si>
-    <t>Conserve your forces and energies by keeping them concentrated at their strongest point.  You gain more by finding a rich mine and mining it deeper, than by flitting from one shallow mine to another - intensity defeats extensity every time.  When looking for sources of power to elevate you, find the one key patron, the fat cow who will give you milk for a long time to come.</t>
-  </si>
-  <si>
-    <t>Your actions must seem natural and executed with ease.  All the toil and practice that go into them, and also all the clever tricks, must be concealed.  When you act, act effortlessly, as if you could do much more. Avoid the temptation of revealing how hard you work - it only raises questions.  Teach no one your tricks or they will be used against you.</t>
-  </si>
-  <si>
-    <t>Never seem to be in a hurry - hurrying betrays a lack of control over yourself, and over time.  Always seem patient, as if you know that everything will come to you eventually. Become a detective of the right moment; sniff out the spirit of the times, the trends that will carry you to power.  Learn to stand back when the time is not yet ripe, and to strike fiercely when it has reached fruition.</t>
-  </si>
-  <si>
-    <t>Striking imagery and grand symbolic gestures create the aura of power - everyone responds to them.  Stage spectacles for those around you, then full of arresting visuals and radiant symbols that heighten your presence.  Dazzled by appearances, no one will notice what you are really doing.</t>
-  </si>
-  <si>
-    <t>The worth of money is not in its possession, but in its use.
-What is offered for free is dangerous - it usually involves either a trick or a hidden obligation.  What has worth is worth paying for. By paying your own way you stay clear of gratitude, guilt, and deceit.  It is also often wise to pay the full price - there are no cutting corners with excellence. Be lavish with your money and keep it circulating, for generosity is a sign and a magnet for power.</t>
-  </si>
-  <si>
-    <t>Trouble can often be traced to a single strong individual - the stirrer, the arrogant underling, the poisoned of goodwill.  If you allow such people room to operate, others will succumb to their influence. Do not wait for the troubles they cause to multiply, do not try to negotiate with them - they are irredeemable.  Neutralize their influence by isolating or banishing them. Strike at the source of the trouble and the sheep will scatter.</t>
   </si>
   <si>
     <t>Decentralize your army to gain mobility and speed.
@@ -1000,26 +761,6 @@
 Break your forces into independent groups that can operate on their own. Give them the spirit of the campaign, a mission to accomplish, and room to run.</t>
   </si>
   <si>
-    <t>Value learning over money.
-Keep expanding your horizons - reading books and materials that go beyond what is required is a good starting point.
-Revert to a feeling of inferiority - when you enter a new environment, your task is to learn and absorb as much as possible.  For that purpose you must try to revert to a childlike feeling of inferiority.  You are full of curiosity.
-Trust the process - push through the point of frustration, trust steady practice to get you through lows.
-Move towards resistance and pain - be your own worst critic, resist the lure of easing up on your focus, and push towards raising your own standards of excellence.
-Apprentice yourself in failure - act on your ideas as early as possible, expose them to the public, and be prepared to fail.  Repeated failure will toughen your spirit and show you with absolute clarity how things must be done.
-Combine the "how" and the "what" - take the extra effort to learn how things are done, not just how they appear, and gain a deeper understanding and feeling for the whole.
-Advance through trial and error - learn as many skills as possible, but only related to your deepest interests.  Find out what work suits you, and what doesn't.  Be comfortable proceeding based on what you like, and when you are ready to settle, ideas and opportunities will present themselves to you.</t>
-  </si>
-  <si>
-    <t>If You Want to Gather Honey, Don't Kick Over the Beehive. 
-Criticism more often is met with resentment than behavioral change. When you don't agree with someone, feel they have done wrong, or need to give someone negative feedback, it's hard not to be critical. However, Carnegie argues we cannot change behavior with threats or punishments. In his classic study, psychologist B.F. Skinner proved that when animals are rewarded for good behavior, they learn faster than animals punished for bad behavior.
-Let's follow Benjamin Franklin's wise advice: "I will speak ill of no man"¦ and speak all the good I know of everybody."</t>
-  </si>
-  <si>
-    <t>The Big Secret of Dealing with People is making everyone feel important. 
-We don't do this with false flattery or brown nosing :  there is nothing worse than an office suck-up. Carnegie argues the best way to make someone feel important is to be curious about them. When you are sitting with a colleague or chatting with someone at a networking event, ask questions that allow you to be sincerely interested.
-Follow Charles Schwab's lead, "I consider my ability to arouse enthusiasm among the men the greatest asset I possess, and the way to develop the best that is in a man is by appreciation and encouragement."</t>
-  </si>
-  <si>
     <t>He Who Can Do This Has the Whole World with Him. 
 Before empathy became a buzzword, Carnegie was all about putting yourself in everyone else's shoes. The best metaphor in this chapter comes from David Lloyd George, former Prime Minister of the United Kingdom. He said he was able to maintain his power because he could "bait the hook to suit the fish." When you want to convince someone to buy your product, go into business with you, or agree with your idea, don't tell them why it will work, tell them why it will benefit them.
 Make Henry Ford's motto your own: "If there is any one secret to success, it lies in the ability to get the other person's point of view and see things from his angle as well as your own."</t>
@@ -1030,34 +771,12 @@
 Quote to post on your workspace: "We are interested in others when they are interested in us." - Publilius Syrus</t>
   </si>
   <si>
-    <t>A Simple Way to Make a Good First Impression. 
-This is the only principle in the entire book that I have some issues with. Carnegie argues that a smile is the best way to show someone: "I like you. You make me happy. I am glad to see you."
-In a professional setting, a smile is not always needed. A warm greeting :  yes! Acknowledgement of someone :  definitely! Avoiding the negative :  sure! But you do not have to walk around the office with a fake smile plastered to your face. It comes across as insincere and is not seen as professional.</t>
-  </si>
-  <si>
     <t>If You Don't Do This, You Are Headed for Trouble. 
 We love hearing the sound of our own name. An easy way to make someone feel appreciated and heard is to show them you remember their name by using it regularly. This also means you have to work to remember names when you hear them. Create a system to remember people's names when you hear them. Or study up before meetings or networking events by looking over the RSVP list.
 Dale Carnegie summarizes this nicely: "The average person is more interested in his or her own name than in all the other names on Earth put together."</t>
   </si>
   <si>
-    <t>How to Interest People. I love to look for people's hot buttons. 
-These are topics of conversations that light up people. You should know all of your colleagues hot buttons :  what do they love to talk about? What do they spend their free time reading about? What gets them talking? Whenever you are with them, try to encourage them to talk about their most passionate interest and try to learn from them. This is the best way to get someone onto your side to show them you are interested in theirs.
-Listen to Teddy Roosevelt: "The royal road to a person's heart is to talk about the things he or she treasures most."</t>
-  </si>
-  <si>
-    <t>How to Make People Like You Instantly. 
-Treat other people in the way you yourself would like to be treated. Carnegie says that whenever you meet someone, you should ask yourself this basic question:
-"What is there about him that I can honestly admire?"
-Practice doing this with everyone you meet and pay special attention to people close to you.</t>
-  </si>
-  <si>
     <t>Never say, "You're wrong"</t>
-  </si>
-  <si>
-    <t>A Sure Way of Making Enemies - and How to Avoid It.
-Every conflict or debate should start with a big dose of humility. We tend to think we are in the right all the time :  immune to silly mistakes. However, if we go through life constantly thinking "I'm right," that makes others instantly wrong if they disagree with you. NO ONE likes to be wrong. Instead, be open to others' opinions. I love Carnegie's script for when you *think* someone is wrong. Say:
-"Well, now, look! I thought otherwise, but I may be wrong. I frequently am. And if I am wrong, I want to be put right. Let's examine the facts."
-Then proceed to discover the facts together.</t>
   </si>
   <si>
     <t>If You're Wrong, Admit It. 
@@ -1069,17 +788,6 @@
   <si>
     <t>The Safety Valve in Handling Complaints. 
 When people do not feel heard, understood or valued, they close up and shut down. If you are dealing with a difficult person, try finding the good in them. Remind them of their best day. La Rochefoucauld wisely said, "If you want enemies, excel your friends; but if you want friends, let your friends excel you."</t>
-  </si>
-  <si>
-    <t>How to Get Cooperation. 
-This is a hard one :  but incredibly important. Carnegie argues that credit should not always be given where it is due. When you can, give up credit, offer praise, highlight someone's else's contribution.
-In the words of Lao Tzu:
-"The reason why rivers and seas receive the homage of a hundred mountain streams is that they keep below them. Thus they are able to reign over all the mountain streams. So the sage, wishing to be above men, putteth himself below them; wishing to be before them, he putteth himself behind them. Thus, though his place be above men, they do not feel his weight; though his place be before them, they do not count it an injury."</t>
-  </si>
-  <si>
-    <t>What Everybody Wants. Sympathy. 
-We all want to make sure that people understand our point of view. In fact, the more you can use someone else's words and tell them about their own opinions the better!
-Carnegie uses a magical phrase:  "I don't blame you one iota for feeling as you do. If I were you, I should undoubtedly feel just as you do."</t>
   </si>
   <si>
     <t>An Appeal That Everybody Likes. 
@@ -1088,162 +796,452 @@
 By appealing to someone's sense of goodness, you often can encourage them to act with good intentions.</t>
   </si>
   <si>
-    <t>The Movies Do It. The Radio Does It. 
-Why Don't You Do It? The more you can make your language, examples and stories "vivid, interesting, dramatic," the more people will listen. We all like a little bit of flare and drama. Don't stick with a boring slide template, make it snazzy. Don't present from a lectern, take some ideas from the best TED Talks. Don't do what everyone else is doing, do something different. This is especially important if you are doing a lot of presentations or public speaking.</t>
-  </si>
-  <si>
     <t>Give the Dog a Good Name. 
 A truth of human nature is that people will be compelled to live up to whatever reputation you attribute to them. When you give someone a positive label or set a high bar they are more likely to clear it. Carnegie summarizes this well, "The average person can be led readily if you have his or her respect and if you show that you respect that person for some kind of ability." Always be looking for someone's natural skills or talents, then remind them of these talents so they use them more often!</t>
   </si>
   <si>
+    <t>The Secret of Socrates. 
+Always try starting an interaction on agreement. What can you and the other person emphatically agree on? What questions can you ask that get the other person to say 'Yes!' or 'Me too!'? If you start in agreement, it is easier to finish with agreement. Carnegie bases his argument on the "Socratic method." His approach to people always was to ask people questions with which they have to agree. This gets people into a 'yes' frame of mind and will make them more open to new ideas later. It also makes 'no's' harder, so people think twice before saying 'no.'</t>
+  </si>
+  <si>
+    <t>PrincipleType</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>How To Win Friends and Influence People</t>
+  </si>
+  <si>
+    <t>The Law Of Human Nature</t>
+  </si>
+  <si>
+    <t>The 48 Laws of Power</t>
+  </si>
+  <si>
+    <t>The 33 Strategies of War</t>
+  </si>
+  <si>
+    <t>Have wide knowledge of multiple fields.
+Never settle into complacency, as if your initial vision represents the endpoint.
+Finally, you must come to embrace slowness as a virtue in itself.
+Imagine yourself years in the future looking back at the work you have done. From that future vantage point, the extra months and years you devoted to the process will not seem painful or laborious at all.</t>
+  </si>
+  <si>
+    <t>Oddly enough, they discovered that what really makes successful entrepreneurs is not the nature of their idea, or the university they went to, but their actual character: their willingness to adapt their idea and take advantage of possibilities they had not first imagined. This is precisely the trait: fluidity of mind. The other essential character trait was supreme tenacity.
+The lesson is simple: what constitutes true creativity is the openness and adaptability of our spirit. When we see or experience something we must be able to look at it from several angles, to see other possibilities beyond the obvious ones.
+The difference then is not in some initial creative power of the brain, but in how we look at the world and the fluidity with which we can reframe what we see. Creativity and adaptability are inseparable.</t>
+  </si>
+  <si>
+    <t>If You Want to Gather Honey, Don't Kick Over the Beehive. 
+Criticism more often is met with resentment than behavioral change. When you don't agree with someone, feel they have done wrong, or need to give someone negative feedback, it's hard not to be critical. However, Carnegie argues we cannot change behavior with threats or punishments. In his classic study, psychologist B.F. Skinner proved that when animals are rewarded for good behavior, they learn faster than animals punished for bad behavior.
+Let's follow Benjamin Franklin's wise advice: "I will speak ill of no man and speak all the good I know of everybody."</t>
+  </si>
+  <si>
+    <t>An Easy Way to Become a Good Conversationalist. 
+We often think that being a good conversationalist means coming up with witty stories and funny jokes. But, actually, we like to hear ourselves talk. If you want to be seen as interesting, ask interesting questions and try to get the other person to open up. This doesn't mean you have to sit listening in silence. I like to think about listening as an active experience. Ask questions, use 'aha's' and 'wow's' and give them nonverbal encouragement.
+Are you really addicted to talking? Or worse, are you an interrupter? You might consider taking a Vow of Silence.</t>
+  </si>
+  <si>
+    <t>How to Make People Like You Instantly. 
+Treat other people in the way you yourself would like to be treated. Carnegie says that whenever you meet someone, you should ask yourself this basic question:
+"What is there about them that I can honestly admire?"
+Practice doing this with everyone you meet and pay special attention to people close to you.</t>
+  </si>
+  <si>
+    <t>You Can't Win an Argument. 
+Carnegie makes a great argument about arguing: you can't win. Even if you have the best possible stances and evidence, if you shoot down your opponent or make them feel wrong, they will resent you. So, even if you technically 'win,' you actually lose. This is especially hard in the age of data, instant Googling and research. If you want to prove someone wrong, see how you can discover what is right together.
+Abraham Lincoln wisely said, "No man who is resolved to make the most of himself can spare the time for personal contention."</t>
+  </si>
+  <si>
+    <t>Speak through your work - be efficient, detail-oriented, and make what you write or present clear and easy to follow, and this will show your care for the audience or public at large.
+Craft the appropriate persona - people will judge you based on your outward appearance - be aware of this and plan for it.
+See yourself as others see you - look at negative events in your past and dissect these occurrences. What patterns can we observe that reveal flaws in our character? Seek opinions from those you trust about your behaviour as well, and begin to cultivate the ability to see yourself as you really are.
+Suffer fools gladly - they are simply part of life, like rocks or furniture. Smile at their antics, tolerate their presence, and avoid the madness of trying to change them.</t>
+  </si>
+  <si>
+    <t>Value learning over money.
+Keep expanding your horizons - reading books and materials that go beyond what is required is a good starting point.
+Revert to a feeling of inferiority - when you enter a new environment, your task is to learn and absorb as much as possible. For that purpose you must try to revert to a childlike feeling of inferiority. You are full of curiosity.
+Trust the process - push through the point of frustration, trust steady practice to get you through the lows.
+Move towards resistance and pain - be your own worst critic, resist the lure of easing up on your focus, and push towards raising your own standards of excellence.
+Apprentice yourself in failure - act on your ideas as early as possible, expose them to the public, and be prepared to fail. Repeated failure will toughen your spirit and show you with absolute clarity how things must be done.
+Combine the "how" and the "what" - take the extra effort to learn how things are done, not just how they appear, and gain a deeper understanding and feeling for the whole.
+Advance through trial and error - learn as many skills as possible, but only related to your deepest interests. Find out what work suits you, and what doesn't. Be comfortable proceeding based on what you like, and when you are ready to settle, ideas and opportunities will present themselves to you.</t>
+  </si>
+  <si>
+    <t>The Big Secret of Dealing with People is making everyone feel important. 
+We don't do this with false flattery or brown nosing: there is nothing worse than an office suck-up. Carnegie argues the best way to make someone feel important is to be curious about them. When you are sitting with a colleague or chatting with someone at a networking event, ask questions that allow you to be sincerely interested.
+Follow Charles Schwab's lead, "I consider my ability to arouse enthusiasm among the men the greatest asset I possess, and the way to develop the best that is in a man is by appreciation and encouragement."</t>
+  </si>
+  <si>
+    <t>A Simple Way to Make a Good First Impression. 
+Carnegie argues that a smile is the best way to show someone: "I like you. You make me happy. I am glad to see you."
+In a professional setting, a smile is not always needed. A warm greeting: yes! Acknowledgement of someone: definitely! Avoiding the negative: sure! But you do not have to walk around the office with a fake smile plastered to your face. It comes across as insincere and is not seen as professional.</t>
+  </si>
+  <si>
+    <t>How to Interest People. Look for people's hot buttons. 
+These are topics of conversations that light up people. You should know all of your colleagues hot buttons: what do they love to talk about? What do they spend their free time reading about? What gets them talking? Whenever you are with them, try to encourage them to talk about their most passionate interest and try to learn from them. This is the best way to get someone onto your side to show them you are interested in theirs.
+Listen to Teddy Roosevelt: "The royal road to a person's heart is to talk about the things he or she treasures most."</t>
+  </si>
+  <si>
+    <t>A Sure Way of Making Enemies - and How to Avoid It.
+Every conflict or debate should start with a big dose of humility. We tend to think we are in the right all the time: immune to silly mistakes. However, if we go through life constantly thinking "I'm right," that makes others instantly wrong if they disagree with you. NO ONE likes to be wrong. Instead, be open to others' opinions. Carnegie's script for when you *think* someone is wrong. Say:
+"Well, now, look! I thought otherwise, but I may be wrong. I frequently am. And if I am wrong, I want to be put right. Let's examine the facts."
+Then proceed to discover the facts together.</t>
+  </si>
+  <si>
+    <t>The High Road to a Man's Reason is kindness. 
+No matter how angry, frustrated or upset you are: never start on a bad foot. There is almost no way to recover from a bad start. Woodrow Wilson put it best:
+"If you come at me with your fists doubled, I think I can promise you that mine will double as fast as yours; but if you come to me and say, 'Let us sit down and take counsel together, and, if we differ from one another, understand why it is that we differ from one another, just what the points at issue are,' we will presently find that we are not so far apart after all, that the points on which we differ are few and the points on which we agree are many, and that if we only have the patience and the candor and the desire to get together, we will get together."</t>
+  </si>
+  <si>
+    <t>How to Get Cooperation. 
+This is a hard one: but incredibly important. Carnegie argues that credit should not always be given where it is due. When you can, give up credit, offer praise, highlight someone's else's contribution.
+In the words of Lao Tzu:
+"The reason why rivers and seas receive the homage of a hundred mountain streams is that they keep below them. Thus they are able to reign over all the mountain streams. So the sage, wishing to be above men, putteth himself below them; wishing to be before them, he putteth himself behind them. Thus, though his place be above men, they do not feel his weight; though his place be before them, they do not count it an injury."</t>
+  </si>
+  <si>
+    <t>What Everybody Wants. Sympathy. 
+We all want to make sure that people understand our point of view. In fact, the more you can use someone else's words and tell them about their own opinions the better!
+Carnegie uses a magical phrase: "I don't blame you one iota for feeling as you do. If I were you, I should undoubtedly feel just as you do."</t>
+  </si>
+  <si>
+    <t>If You Must Find Fault, This Is the Way to Begin. 
+What has someone done well? Where can you agree? What is working? Carnegie encourages readers to start all interactions: especially ones that have the potential for disagreement, with honest appreciation.</t>
+  </si>
+  <si>
+    <t>How to Spur Men on to Success. 
+While Carnegie encourages readers to be careful and hold back criticism or judgment, he says to lavish genuine praise whenever it is warranted. Here are some ideas:
+Thank people for their work.
+Compliment any exceptional traits or qualities.
+Be specific with your compliments: and don't give everyone the same compliments!</t>
+  </si>
+  <si>
+    <t>Use the wisdom, knowledge, and legwork of other people to further your own cause. Not only will such assistance save you valuable time and energy, it will give you a godlike aura of efficiency and speed. In the end, your helpers will be forgotten and you will be remembered. Never do yourself what others can do for you.</t>
+  </si>
+  <si>
+    <t>For negotiations or meetings, it is always wise to lure others into your territory, or the territory of your choice. You have your bearings, while they see nothing familiar and are subtly placed on the defensive.
+When you force the other person to act, you are the one in control. It is always better to make your opponent come to you, abandoning his own plans in the process. Lure him with fabulous gains - then attack. You hold the cards.</t>
+  </si>
+  <si>
+    <t>Any momentary triumph you think gained through argument is really a Pyrrhic victory: The resentment and ill will you stir up is stronger and lasts longer than any momentary change of opinion. It is much more powerful to get others to agree with you through your actions, without saying a word. Demonstrate, do not explicate.</t>
+  </si>
+  <si>
+    <t>You can die from someone else's misery - emotional states are as infectious as disease. You may feel you are helping the drowning man but you are only precipitating your own disaster. The unfortunate sometimes draw misfortune on themselves; they will also draw it on you. Associate with the happy and fortunate instead.
+When you suspect you are in the presence of an infector, don't argue, don't try to help, don't pass the person on to your friends, or you will become enmeshed. Flee the infector's presence or suffer the consequences.</t>
+  </si>
+  <si>
+    <t>To maintain your independence you must always be needed and wanted. The more you are relied on, the more freedom you have. Make people depend on you for their happiness and prosperity and you have nothing to fear. Never teach them enough so that they can do without you.</t>
+  </si>
+  <si>
+    <t>One sincere and honest move will cover over dozens of dishonest ones. Open-hearted gestures of honesty and generosity bring down the guard of even the most suspicious people. Once your selective honesty opens a hole in their armor, you can deceive and manipulate them at will. A timely gift - a Trojan horse - will serve the same purpose.</t>
+  </si>
+  <si>
+    <t>If you need to turn to an ally for help, do not bother to remind him of your past assistance and good deeds. He will find a way to ignore you. Instead, uncover something in your request, or in your alliance with him, that will benefit him, and emphasize it out of all proportion. He will respond enthusiastically when he sees something to be gained for himself.</t>
+  </si>
+  <si>
+    <t>Knowing about your rival is critical. Use spies to gather valuable information that will keep you a step ahead. Better still: Play the spy yourself. In polite social encounters, learn to probe. Ask indirect questions to get people to reveal their weaknesses and intentions. There is no occasion that is not an opportunity for artful spying.</t>
+  </si>
+  <si>
+    <t>All great leaders since Moses have known that a feared enemy must be crushed completely. (Sometimes they have learned this the hard way.) If one ember is left alight, no matter how dimly it smolders, a fire will eventually break out. More is lost through stopping halfway than through total annihilation: The enemy will recover and will seek revenge. Crush him, not only in body but in spirit.</t>
+  </si>
+  <si>
+    <t>Humans are creatures of habit with an insatiable need to see familiarity in other people's actions. Your predictability gives them a sense of control. Turn the tables: Be deliberately unpredictable. Behavior that seems to have no consistency or purpose will keep them off-balance, and they will wear themselves out trying to explain your moves. Taken to an extreme, this strategy can intimidate and terrorize.
+Too much unpredictability will be seen as a sign of indecisiveness, or even of some more serious psychic problem. Patterns are powerful, and you can terrify people by disrupting them. Such power should only be used judiciously.</t>
+  </si>
+  <si>
+    <t>The world is dangerous and enemies are everywhere - everyone has to protect themselves. A fortress seems the safest. But isolation exposes you to more dangers than it protects you from - it cuts you off from valuable information, it makes you conspicuous and an easy target. Better to circulate among people, find allies, mingle. You are shielded from your enemies by the crowd.</t>
+  </si>
+  <si>
+    <t>Given how important the idea of intelligence is to most people's vanity, it is critical never inadvertently to insult or impugn a person's brain power.
+No one likes feeling stupider than the next person. The trick, then, is to make your victims feel smart - and not just smart, but smarter than you are. Once convinced of this, they will never suspect that you may have ulterior motives.</t>
+  </si>
+  <si>
+    <t>Conserve your forces and energies by keeping them concentrated at their strongest point. You gain more by finding a rich mine and mining it deeper, than by flitting from one shallow mine to another - intensity defeats extensity every time. When looking for sources of power to elevate you, find the one key patron, the fat cow who will give you milk for a long time to come.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The perfect courtier thrives in a world where everything revolves around power and political dexterity. He has mastered the art of indirection; he flatters, yields to superiors, and asserts power over others in the most oblique and graceful manner. Learn and apply the laws of courtiership and there will be no limit to how far you can rise in the court. </t>
+  </si>
+  <si>
+    <t>You must seem a paragon of civility and efficiency: Your hands are never soiled by mistakes and nasty deeds. Maintain such a spotless appearance by using others as scapegoats and cat's-paws to disguise your involvement.</t>
+  </si>
+  <si>
+    <t>People have an overwhelming desire to believe in something. Become the focal point of such desire by offering them a cause, a new faith to follow. Keep your words vague but full of promise; emphasize enthusiasm over rationality and clear thinking. Give your new disciples rituals to perform, ask them to make sacrifices on your behalf. In the absence of organized religion and grand causes, your new belief system will bring you untold power.</t>
+  </si>
+  <si>
+    <t>Lions circle the hesitant prey.
+Boldness strikes fear, fear creates authority.
+Going halfway with half a heart digs a deeper grave.
+Hesitation creates gaps, boldness obliterates them.
+Audacity separates you from the herd.
+When you are as small and obscure as David was, you must find a Goliath to attack. The larger the target, the more attention you gain.
+Timidity is dangerous: Better to enter with boldness. Any mistakes you commit through audacity are easily corrected with more audacity. Everyone admires the bold; no one honors the timid.</t>
+  </si>
+  <si>
+    <t>The ending is everything. Plan all the way to it, taking into account all the possible consequences, obstacles, and twists of fortune that might reverse your hard work and give the glory to others. By planning to the end you will not be overwhelmed by circumstances and you will know when to stop. Gently guide fortune and help determine the future by thinking far ahead.</t>
+  </si>
+  <si>
+    <t>Your actions must seem natural and executed with ease. All the toil and practice that go into them, and also all the clever tricks, must be concealed. When you act, act effortlessly, as if you could do much more. Avoid the temptation of revealing how hard you work - it only raises questions. Teach no one your tricks or they will be used against you.</t>
+  </si>
+  <si>
+    <t>Everyone has a weakness, a gap in the castle wall. That weakness is usually an insecurity, an uncontrollable emotion or need; it can also be a small secret pleasure. Either way, once found it is a thumbscrew you can turn to your advantage.</t>
+  </si>
+  <si>
+    <t>The way you carry yourself will often determine how you are treated; In the long run, appearing vulgar or common will make people disrespect you. For a king respects himself and inspires the same sentiment in others. By acting regally and confident of your powers, you make yourself seem destined to wear a crown.</t>
+  </si>
+  <si>
+    <t>Striking imagery and grand symbolic gestures create the aura of power - everyone responds to them. Stage spectacles for those around you, then full of arresting visuals and radiant symbols that heighten your presence. Dazzled by appearances, no one will notice what you are really doing.</t>
+  </si>
+  <si>
+    <t>If you make a show of going against the times, flaunting your unconventional ideas and unorthodox ways, people will think that you only want attention and that you look down upon them. They will find a way to punish you for making them feel inferior. It is far safer to blend in and nurture the common touch. Share your originality only with tolerant friends and those who are sure to appreciate your uniqueness.</t>
+  </si>
+  <si>
+    <t>Anger and emotion are strategically counterproductive. You must always stay calm and objective. But if you can make your enemies angry while staying calm yourself, you gain a decided advantage. Put your enemies off-balance: Find the chink in their vanity through which you can rattle them and you hold the strings.</t>
+  </si>
+  <si>
+    <t>The worth of money is not in its possession, but in its use.
+What is offered for free is dangerous - it usually involves either a trick or a hidden obligation. What has worth is worth paying for. By paying your own way you stay clear of gratitude, guilt, and deceit. It is also often wise to pay the full price - there are no cutting corners with excellence. Be lavish with your money and keep it circulating, for generosity is a sign and a magnet for power.</t>
+  </si>
+  <si>
+    <t>What happens first always appears better and more original than what comes after. If you succeed a great man or have a famous parent, you will have to accomplish double their achievements to outshine them. Do not get lost in their shadow, or stuck in a past, not of your own making: Establish your own name and identity by changing course. Slay the overbearing father, disparage his legacy, and gain power by shining in your own way.</t>
+  </si>
+  <si>
+    <t>Trouble can often be traced to a single strong individual - the stirrer, the arrogant underling, the poisoned of goodwill. If you allow such people room to operate, others will succumb to their influence. Do not wait for the troubles they cause to multiply, do not try to negotiate with them - they are irredeemable. Neutralize their influence by isolating or banishing them. Strike at the source of the trouble and the sheep will scatter.</t>
+  </si>
+  <si>
+    <t>Coercion creates a reaction that will eventually work against you. You must seduce others into wanting to move in your direction. A person you have seduced becomes your loyal pawn. And the way to seduce others is to operate on their individual psychologies and weaknesses. Soften up the resistant by working on their emotions, playing on what they hold dear and what they fear. Ignore the hearts and minds of others and they will grow to hate you.</t>
+  </si>
+  <si>
+    <t>The mirror reflects reality, but it is also the perfect tool for deception: When you mirror your enemies, doing exactly as they do, they cannot figure out your strategy. The Mirror Effect mocks and humiliates them, making them overreact. By holding up a mirror to their psyches, you seduce them with the illusion that you share their values; by holding up a mirror to their actions, you teach them a lesson. Few can resist the power of the Mirror Effect.</t>
+  </si>
+  <si>
+    <t>Everyone understands the need for change in the abstract, but on the day-to-day level, people are creatures of habit. Too much innovation is traumatic and will lead to revolt. If you are new to a position of power, or an outsider trying to build a power base, make a show of respecting the old way of doing things. If change is necessary, make it feel like a gentle improvement on the past.</t>
+  </si>
+  <si>
+    <t>Appearing better than others is always dangerous, but most dangerous of all is to appear to have no faults or weaknesses. Envy creates silent enemies. It is smart to occasionally display defects, and admit to harmless vices, in order to deflect envy and appear more human and approachable. Only gods and the dead can seem perfect with impunity.
+Do not try to help or do favors for those who envy you; they will think you are condescending to them.</t>
+  </si>
+  <si>
+    <t>The moment of victory is often the moment of greatest peril. In the heat of victory, arrogance and overconfidence can push you past the goal you had aimed for, and by going too far, you make more enemies than you defeat. Do not allow success to go to your head. There is no substitute for strategy and careful planning. Set a goal, and when you reach it, stop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By taking a shape, by having a visible plan, you open yourself to attack. Instead of taking a form for your enemy to grasp, keep yourself adaptable and on the move. Accept the fact that nothing is certain and no law is fixed. The best way to protect yourself is to be as fluid and formless as water; never bet on stability or lasting order. Everything changes. </t>
+  </si>
+  <si>
+    <t>The Movies Do It. The Radio Does It. Why Don't You Do It? 
+The more you can make your language, examples and stories "vivid, interesting, dramatic," the more people will listen. We all like a little bit of flare and drama. Don't stick with a boring slide template, make it snazzy. Don't present from a lectern, take some ideas from the best TED Talks. Don't do what everyone else is doing, do something different. This is especially important if you are doing a lot of presentations or public speaking.</t>
+  </si>
+  <si>
+    <t>How to Criticize - and Not Be Hated for It. 
+When you must criticize, try finding a way to do so indirectly. This is similar to the Poop Sandwich Method: you have to be able to give hard news sometimes. When giving a Poop Sandwich, always use 'and' not 'but.' Most people begin their criticism with appreciation, but then follow it with the word "but" and go into the poopy news, such as "You've been working so hard and we really appreciate that, but..." Once someone hears the "but", it makes them question the sincerity of the appreciation. Try replacing the word "but" with "and". Example: "You've been working so hard and we really appreciate that, and we have some ideas on how to make all of your effort pay off even more. Here's what we were thinking..."</t>
+  </si>
+  <si>
     <t>Law: Many people are narcissists i.e. focus on and admire themselves more than others. This hinders their success when interacting with others. Narcissists can be dangerous.
-Example: Joseph Stalin "” premier of the Soviet Union "” was a very charming and influential person. He was also a narcissist who killed many people during his reign. Leo Tolstoy "” a Russian novelist "” and his wife Sonya were both narcissists. Their relationship was complicated. Lack of empathy made the partners retreat deeper and deeper into their own defensive positions.
+Example: Joseph Stalin, premier of the Soviet Union, was a very charming and influential person. He was also a narcissist who killed many people during his reign. Leo Tolstoy, a Russian novelist, and his wife Sonya were both narcissists. Their relationship was complicated. Lack of empathy made the partners retreat deeper and deeper into their own defensive positions.
 Advice: You need to transform self-love into empathy. This will make you more successful in your group.</t>
   </si>
   <si>
-    <t>Law: People tend to wear the mask that shows them in the best possible light. They hide their true personality.
-Example: Milton Erickson "” an American psychiatrist and psychologist of 20th century "” was paralysed when he was
-young and became a master reader of people body language.
-Advice: You must master the body language by transforming yourself into a superior reader of men and women. At the same time you must learn how to present the best front and play your role to maximum effect.</t>
-  </si>
-  <si>
     <t>Law: People never do something just once. They will inevitably repeat their bad behavior.
-Example: Howard Hughes Jr. "” an American business magnate, investor, record-setting pilot, engineer, film director, and philanthropist "” had a weak character since his childhood. He managed to disguise it in his early career which brought him success. However it manifested later in his life and resulted in many failures including Hughes Aircraft Company.
+Example: Howard Hughes Jr., an American business magnate, investor, record-setting pilot, engineer, film director, and philanthropist, had a weak character since his childhood. He managed to disguise it in his early career which brought him success. However it manifested later in his life and resulted in many failures including Hughes Aircraft Company.
 Advice: Train yourself to look deep within people and see their character. Always gravitate toward those who display signs of strength, and avoid the many toxic types out there.</t>
   </si>
   <si>
     <t>Law: People continually desire to possess what they don't have.
-Example: Coco Chanel "” a French fashion designer and business woman "” became so successful not only because she created great products but because she understood that people desire what they don't have and created an air of mystery around her work.
+Example: Coco Chanel, a French fashion designer and business woman, became so successful not only because she created great products but because she understood that people desire what they don't have and created an air of mystery around her work.
 Advice: Become an elusive object of desire.</t>
   </si>
   <si>
     <t>Law: People tend to overreact to present circumstances and ignore what will happen in the future.
-Example: The South Sea Company "” a British joint-stock company founded in 1711 "” became known as the South Sea Bubble. It was obvious that the company can't succeed long-term but it didn't stop many people from investing in its shares.
+Example: The South Sea Company, a British joint-stock company founded in 1711, became known as the South Sea Bubble. It was obvious that the company can't succeed long-term but it didn't stop many people from investing in its shares.
 Advice: When making decisions think about the near and far future.</t>
   </si>
   <si>
     <t>Law: People don't like when someone is trying to change their opinion.
-Example: Lyndon Johnson "” the 36th president of the United States "” gained his influence and power by focusing on others, letting them do the talking, letting them be the stars of the show.
+Example: Lyndon Johnson, the 36th president of the United States, gained his influence and power by focusing on others, letting them do the talking, letting them be the stars of the show.
 Advice: Soften people's resistance by confirming their self-opinion.</t>
   </si>
   <si>
     <t>Law: Our attitude determines much of what happens in our life.
-Example: Anton Chekhov "” a Russian playwright and short-story writer "” had a tough childhood but in spite of that was able to change his life by changing his view of the world from negative to positive.
+Example: Anton Chekhov, a Russian playwright and short-story writer, had a tough childhood but in spite of that was able to change his life by changing his view of the world from negative to positive.
 Advice: Change your circumstances by changing your attitude.</t>
   </si>
   <si>
     <t>Law: People are rarely who they seem to be. Lurking beneath their polite, affable exterior is inevitably a dark, shadow side consisting of the insecurities and the aggressive, selfish impulses they repress and carefully conceal from public view.
-Example: Richard Nixon "” the 37th president of the United States "” always had a positive image in the public. Everything changed after the Watergate scandal which revealed his hidden personality.
+Example: Richard Nixon, the 37th president of the United States, always had a positive image in the public. Everything changed after the Watergate scandal which revealed his hidden personality.
 Advice: Be aware of your own dark side. Control and channel the creative energies that lurk in your unconscious. By integrating the dark side into your personality, you will be a more complete human and will radiate an authenticity that will draw people to you.</t>
   </si>
   <si>
     <t>Law: People are envious.
-Example: Mary Shelley "” author of the novel Frankenstein "” was betrayed by her close friend who envied her.
+Example: Mary Shelley, author of the novel Frankenstein, was betrayed by her close friend who envied her.
 Advice: Learn to deflect envy by drawing attention away from yourself. Develop your sense of self-worth from internal standards and not incessant comparisons.</t>
   </si>
   <si>
-    <t>Law: Even a small measure of success can elevate our natural grandiosity "” an unrealistic sense of superiority, a sustained view of oneself as better than others. This can make us lose contact with reality and make irrational decisions.
+    <t>Law: Even a small measure of success can elevate our natural grandiosity, an unrealistic sense of superiority, a sustained view of oneself as better than others. This can make us lose contact with reality and make irrational decisions.
 Example: Michael Eisner had to resign from the CEO position of The Walt Disney Company. In the author's opinion the cause is Eisner's grandiosity elevated by previous successes.
 Advice: Counteract the pull of grandiosity by maintaining a realistic assessment of yourself and your limits. Tie any feelings of greatness to your work, your achievements, and your contributions to society.</t>
   </si>
   <si>
-    <t>Law: We have a side to our character that we are generally unaware of "” our social personality, the different person we become when we operate in groups of people. In the group setting, we unconsciously imitate what others are saying and doing. We think differently, more concerned with fitting in and believing what others believe. We feel different emotions, infected by the group mood. We are more prone to taking risks, to acting irrationally, because everyone else is.
+    <t>Law: We have a side to our character that we are generally unaware of, our social personality, the different person we become when we operate in groups of people. In the group setting, we unconsciously imitate what others are saying and doing. We think differently, more concerned with fitting in and believing what others believe. We feel different emotions, infected by the group mood. We are more prone to taking risks, to acting irrationally, because everyone else is.
 Example: Gao Yuan tells a story in his book Born Red showed that people in groups behave emotional and excited. They don't engage in nuanced thinking and deep analysis.
 Advice: Develop self-awareness and a superior understanding of the changes that occur in us in groups. With such intelligence, we can become superior social actors, able to outwardly fit in and cooperate with others on a high level, while retaining our independence and rationality.</t>
   </si>
   <si>
     <t>Law: People are always ambivalent about those in power. They want to be led but also to feel free; they want to be protected and enjoy prosperity without making sacrifices; they both worship the king and want to kill him. When you are the leader of a group, people are continually prepared to turn on you the moment you seem weak or experience a setback.
-Example: Elizabeth I "” Queen of England and Ireland in 16th century "” had to constantly prove herself as the leader of the country. She never relied on her royal blood for this.
+Example: Elizabeth I, Queen of England and Ireland in 16th century, had to constantly prove herself as the leader of the country. She never relied on her royal blood for this.
 Advice: Authority is the delicate art of creating the appearance of power, legitimacy, and fairness while getting people to identify with you as a leader who is in their service. If you want to lead, you must master this art from early on in your life.</t>
   </si>
   <si>
     <t>Law: On the surface, the people around you appear so polite and civilized. But beneath the mask, they are all inevitably dealing with frustrations. They have a need to influence people and gain power over circumstances. Feeling blocked in their endeavors, they often try to assert themselves in manipulative ways that catch you by surprise. And then there are those whose need for power and impatience to obtain it are greater than others. They turn particularly aggressive, getting their way by intimidating people, being relentless and willing to do almost anything.
-Example: John D. Rockefeller "” American oil industry business magnate "” used aggressive strategies to gain power and control.
-Advice: You must recognize the signs "” the past patterns of behavior, the obsessive need to control everything in their environment "” that indicate the dangerous types. They depend on making you emotional "” afraid, angry "” and unable to think straight. Do not give them this power. When it comes to your own aggressive energy, learn to tame and channel it for productive purposes "” standing up for yourself, attacking problems with relentless energy, realizing great ambitions.</t>
+Example: John D. Rockefeller, American oil industry business magnate, used aggressive strategies to gain power and control.
+Advice: You must recognize the signs, the past patterns of behavior, the obsessive need to control everything in their environment, that indicate the dangerous types. They depend on making you emotional, afraid, angry, and unable to think straight. Do not give them this power. When it comes to your own aggressive energy, learn to tame and channel it for productive purposes, standing up for yourself, attacking problems with relentless energy, realizing great ambitions.</t>
   </si>
   <si>
     <t>Law: Most people spend their lives avoiding the thought of death.
-Example: Mary Flannery O'Connor "” an American novelist and short story writer "” was diagnosed with systemic lupus erythematosus when she was 27. Her proximity to death was a call to stir herself to action, to feel a sense of urgency, to deepen her religious faith and spark her sense of wonder at all mysteries and uncertainties of life. She used the closeness of death to teach her what really matters and to help her steer clear of the petty squabbles and concerns that plagued others. She used it to anchor herself in the present, to make her appreciate every moment and every encounter.
+Example: Mary Flannery O'Connor, an American novelist and short story writer, was diagnosed with systemic lupus erythematosus when she was 27. Her proximity to death was a call to stir herself to action, to feel a sense of urgency, to deepen her religious faith and spark her sense of wonder at all mysteries and uncertainties of life. She used the closeness of death to teach her what really matters and to help her steer clear of the petty squabbles and concerns that plagued others. She used it to anchor herself in the present, to make her appreciate every moment and every encounter.
 Advice: The inevitability of death should be continually on our minds. Understanding the shortness of life fills us with a sense of purpose and urgency to realize our goals. Training ourselves to confront and accept this reality makes it easier to manage the inevitable setbacks, separations, and crises in life. It gives us a sense of proportion, of what really matters in this brief existence of ours. Most people continually look for ways to separate themselves from others and feel superior. Instead, we must see the mortality in everyone, how it equalizes and connects us all. By becoming deeply aware of our mortality, we intensify our experience of every aspect of life.</t>
   </si>
   <si>
-    <t>But hire a former enemy and he will be more loyal than a friend, because he has more to prove. In fact, you have more to fear from friends than from enemies. If you have no enemies, find a way to make them
-Since honesty rarely strengthens friendship, you may never know how a friend truly feels. Friends will say that they love your poetry, adore your music, envy your taste in clothes"” maybe they mean it, often they do not.
+    <t>Law: People tend to wear the mask that shows them in the best possible light. They hide their true personality.
+Example: Milton Erickson, an American psychiatrist and psychologist of 20th century, was paralysed when he was
+young and became a master reader of people's body language.
+Advice: You must master the body language by transforming yourself into a superior reader of men and women. At the same time you must learn how to present the best front and play your role to maximum effect.</t>
+  </si>
+  <si>
+    <t>Law: All of us have masculine and feminine qualities. But in the need to present a consistent identity in society, we tend to repress these qualities, overidentifying with the masculine or feminine role expected of us. Thereby we lose valuable dimensions to our character.
+Example: Caterina Sforza became an Italian noblewoman and Countess of Forli and Lady of Imola. Such titles were unusual for women in her time. In the author's opinion her masculine qualities helped her to achieve this.
+Advice: You must become aware of these lost masculine or feminine traits and slowly reconnect to them, unleashing creative powers in the process.</t>
+  </si>
+  <si>
+    <t>Hire a former enemy and he will be more loyal than a friend, because he has more to prove. In fact, you have more to fear from friends than from enemies. If you have no enemies, find a way to make them
+Since honesty rarely strengthens friendship, you may never know how a friend truly feels. Friends will say that they love your poetry, adore your music, envy your taste in clothes - maybe they mean it, often they do not.
 The key to power, then, is the ability to judge who is best able to further your interests in all situations. Keep friends for friendship, but work with the skilled and competent.</t>
   </si>
   <si>
     <t>Use decoyed objects and desires and red herrings to throw people off the scent
-Hide your intentions not by closing up (with the risk of appearing secretive, and making people suspicious) but by talking endlessly about your desires and goals"” just not your real ones. You will kill three birds with one stone: You appear friendly, open, and trusting; you conceal your intentions; and you send your rivals on time-consuming wild-goose chases.
+Hide your intentions not by closing up (with the risk of appearing secretive, and making people suspicious) but by talking endlessly about your desires and goals - just not your real ones. You will kill three birds with one stone: You appear friendly, open, and trusting; you conceal your intentions; and you send your rivals on time-consuming wild-goose chases.
 Use smoke screens to disguise your actions. This derives from a simple truth: people can only focus on one thing at a time. It is really too difficult for them to imagine that the bland and harmless person they are dealing with is simultaneously setting up something else
 As Kierkegaard wrote, "The world wants to be deceived."</t>
   </si>
   <si>
-    <t>One oft-told tale about Kissinger"¦ involved a report that Winston Lord had worked on for days. After giving it to Kissinger, he got it back with the notation, "Is this the best you can do?" Lord rewrote and polished and finally resubmitted it; back it came with the same curt question. After redrafting it one more time"” and once again getting the same question from Kissinger-Lord snapped, "Damn it, yes, it's the best I can do. " To which Kissinger replied: "Fine, then I guess I'll read it this time. "
+    <t>Be the master of your own image rather than letting others define it for you.
+The world wants to assign you a role in life. And once you accept that role you are doomed.
+Remake yourself into a character of power. Working on yourself like clay should be one of your greatest and most pleasurable life tasks.
+The first step in the process of self-creation is self-consciousness - being aware of yourself as an actor and taking control of your appearance and emotions.
+The second step in the process of self-creation is a variation on the George Sand strategy: the creation of a memorable character, one that compels attention, that stands out above the other players on the stage.</t>
+  </si>
+  <si>
+    <t>People rarely believe that their problems arise from their own misdeeds and stupidity. Someone or something out there is to blame - the other, the world, the gods - and so salvation comes from the outside as well.
+The truth is often avoided because it is ugly and unpleasant. Never appeal to truth and reality unless you are prepared for the anger that comes for disenchantment. Life is so harsh and distressing that people who can manufacture romance or conjure up fantasy are like oases in the desert: Everyone flocks to them. There is great power in tapping into the fantasies of the masses.</t>
+  </si>
+  <si>
+    <t>Remember: You choose to let things bother you. You can just as easily choose not to notice the irritating offender, to consider the matter trivial and unworthy of your interest. That is the powerful move.
+Desire often creates paradoxical effects: The more you want something, the more you chase after it, the more it eludes you. The more interest you show, the more you repel the object of your desire. This is because your interest is too strong - it makes people awkward, even fearful. Uncontrollable desire makes you seem weak, unworthy, pathetic.
+By acknowledging a petty problem you give it existence and credibility. The more attention you pay an enemy, the stronger you make him; and a small mistake is often made worse and more visible when you try to fix it. It is sometimes best to leave things alone. If there is something you want but cannot have, show contempt for it. The less interest you reveal, the more superior you seem.</t>
+  </si>
+  <si>
+    <t>One oft-told tale about Kissinger involved a report that Winston Lord had worked on for days. After giving it to Kissinger, he got it back with the notation, "Is this the best you can do?" Lord rewrote and polished and finally resubmitted it; back it came with the same curt question. After redrafting it one more time - and once again getting the same question from Kissinger-Lord snapped, "Damn it, yes, it's the best I can do." To which Kissinger replied: "Fine, then I guess I'll read it this time."
 Persons who cannot control his words shows that he cannot control himself, and is unworthy of respect. But the human tongue is a beast that few can master. It strains constantly to break out of its cage, and if it is not tamed, it will run wild and cause you grief. Power cannot accrue to those who squander their treasure of words.
 Power is in many ways a game of appearances, and when you say less than necessary, you inevitably appear greater and more powerful than you are.
 Learn the lesson: Once the words are out, you cannot take them back. Keep them under control. Be particularly careful with sarcasm: The momentary satisfaction you gain with your biting words will be outweighed by the price you pay.</t>
   </si>
   <si>
-    <t>Be the master of your own image rather than letting others define it for you.
-The world wants to assign you a role in life. And once you accept that role you are doomed.
-Remake yourself into a character of power. Working on yourself like clay should be one of your greatest and most pleasurable life tasks.
-The first step in the process of self-creation is self-consciousness"” being aware of yourself as an actor and taking control of your appearance and emotions.
-The second step in the process of self-creation is a variation on the George Sand strategy: the creation of a memorable character, one that compels attention, that stands out above the other players on the stage.</t>
-  </si>
-  <si>
-    <t>You give people a sense of how things will fall apart without you, and you offer them a "choice": I stay away and you suffer the consequences, or I return under circumstances that I dictate.
+    <t>There are many different kinds of people in the world, and you can never assume that everyone will react to your strategies in the same way. Deceive or outmaneuver some people and they will spend the rest of their lives seeking revenge. They are wolves in lamb's clothing. Choose your victims and opponents carefully, then - never offend or deceive the wrong person.</t>
+  </si>
+  <si>
+    <t>You give people a sense of how things will fall apart without you, and you offer them a "choice": I stay away and you suffer the consequences, or I return under circumstances that I dictate.
 Color the choices, propose three or four choices of action for each situation, and would present them in such a way that the one he preferred always seemed the best solution compared to the others.
-Force the resister, Push them to "choose" what you want them to do by appearing to advocate the opposite.
+Force the resister, Push them to "choose" what you want them to do by appearing to advocate the opposite.
 Alter the playing field.
 The shrinking options: A variation on this technique is to raise the price every time the buyer hesitates and another day goes by. This is an excellent negotiating ploy to use on the chronically indecisive, who will fall for the idea that they are getting a better deal today than if they wait till tomorrow.
-The weak man on the precipice: This tactic is similar to "Color the Choices," but with the weak you have to be more aggressive. Work on their emotions"” use fear and terror to propel them into action. Try reason and they will always find a way to procrastinate.
+The weak man on the precipice: This tactic is similar to "Color the Choices," but with the weak you have to be more aggressive. Work on their emotions - use fear and terror to propel them into action. Try reason and they will always find a way to procrastinate.
 Brothers in Crime: You attract your victims to some criminal scheme, creating a bond of blood and guilt between you.
 The horns of a dilemma: The lawyer leads the witnesses to decide between two possible explanations of an event, both of which poke a hole in their story. They have to answer the lawyer's questions, but whatever they say they hurt themselves. The key to this move is to strike quickly: Deny the victim the time to think of an escape. As they wriggle between the horns of the dilemma, they dig their own grave.</t>
   </si>
   <si>
-    <t>People rarely believe that their problems arise from their own misdeeds and stupidity. Someone or something out there is to blame"” the other, the world, the gods"” and so salvation comes from the outside as well.
-The truth is often avoided because it is ugly and unpleasant.  Never appeal to truth and reality unless you are prepared for the anger that comes for disenchantment.  Life is so harsh and distressing that people who can manufacture romance or conjure up fantasy are like oases in the desert:  Everyone flocks to them. There is great power in tapping into the fantasies of the masses.</t>
-  </si>
-  <si>
-    <t>Remember: You choose to let things bother you. You can just as easily choose not to notice the irritating offender, to consider the matter trivial and unworthy of your interest. That is the powerful move.
-Desire often creates paradoxical effects: The more you want something, the more you chase after it, the more it eludes you. The more interest you show, the more you repel the object of your desire. This is because your interest is too strong"” it makes people awkward, even fearful. Uncontrollable desire makes you seem weak, unworthy, pathetic.
-By acknowledging a petty problem you give it existence and credibility.  The more attention you pay an enemy, the stronger you make him; and a small mistake is often made worse and more visible when you try to fix it.  It is sometimes best to leave things alone. If there is something you want but cannot have, show contempt for it. The less interest you reveal, the more superior you seem.</t>
+    <t>Never seem to be in a hurry - hurrying portrays a lack of control over yourself, and over time. Always seem patient, as if you know that everything will come to you eventually. Become a detective of the right moment; sniff out the spirit of the times, the trends that will carry you to power. Learn to stand back when the time is not yet ripe, and to strike fiercely when it has reached fruition.</t>
+  </si>
+  <si>
+    <t>Do not become a sheep in the crowded center: go to the extreme. A dominating polarizing presence has more pull than middle ground men.
+Don't necessarily get into the idea you need to be liked -as in How to Win Friends-, being respected is better, and even being feared. Don't be afraid of battles and enemies either. Your enemies give you a purpose and direction.
+And battles are what will allow you to win.
+And ultimately, it's victory over your enemies that will bring you the most meaningful and lasting popularity.
+Victory over your enemies is the best form of popularity
+Reversal:
+Don't see enemies everywhere, and always keep it for yourself. If you're wrong, nobody will judge you.
+Do like Cortez did. Keep it to yourself, pretend you didn't notice. Let them come more and more on the surface, and when it's obvious to everyone they're enemies, then strike.
+And don't make enemies and pick fights at any time. You don't want to make enemies of everyone.</t>
   </si>
   <si>
     <t>Creating urgency and desperation means to put yourself and the troops in a position where there's no other option but winning.
-It's the "burn your bridges" strategy.
+It's the "burn your bridges" strategy.
 Greene recommends to use the thought of death as your driver to spur you into action.
-I loved this part as I wrote a whole article about it. If you're interested in the subject also read: leveraging mortality.
 Place yourself where your back is against the wall and you have to fight like hell to get out alive.</t>
   </si>
   <si>
-    <t>An Easy Way to Become a Good Conversationalist. 
-We often think that being a good conversationalist means coming up with witty stories and funny jokes. But, actually, we like to hear ourselves talk. If you want to be seen as interesting, ask interesting questions and try to get the other person to open up. This doesn't mean you have to sit listening in silence. I like to think about listening as an active experience. Ask questions, use 'aha's' and 'wow's' and give them nonverbal encouragement.
-Are you really addicted to talking? Or worse, are you an interrupter? You might consider taking a Vow of Silence. I do one of these every year and have found it to be life-changing for my listening ability.</t>
-  </si>
-  <si>
-    <t>You Can't Win an Argument. 
-Carnegie makes a great argument about arguing :  you can't win. Even if you have the best possible stances and evidence, if you shoot down your opponent or make them feel wrong, they will resent you. So, even if you technically 'win,' you actually lose. This is especially hard in the age of data, instant Googling and research. If you want to prove someone wrong, see how you can discover what is right together.
-Abraham Lincoln wisely said, "No man who is resolved to make the most of himself can spare the time for personal contention."</t>
-  </si>
-  <si>
-    <t>The High Road to a Man's Reason is kindness. 
-No matter how angry, frustrated or upset you are :  never start on a bad foot. There is almost no way to recover from a bad start. Woodrow Wilson put it best:
-"If you come at me with your fists doubled, I think I can promise you that mine will double as fast as yours; but if you come to me and say, 'Let us sit down and take counsel together, and, if we differ from one another, understand why it is that we differ from one another, just what the points at issue are,' we will presently find that we are not so far apart after all, that the points on which we differ are few and the points on which we agree are many, and that if we only have the patience and the candor and the desire to get together, we will get together."</t>
-  </si>
-  <si>
-    <t>The Secret of Socrates. 
-Always try starting an interaction on agreement. What can you and the other person emphatically agree on? What questions can you ask that get the other person to say 'Yes!' or 'Me too!'? If you start in agreement, it is easier to finish with agreement. Carnegie bases his argument on the "Socratic method." His approach to people always was to ask people questions with which they have to agree. This gets people into a 'yes' frame of mind and will make them more open to new ideas later. It also makes 'no's' harder, so people think twice before saying 'no.'</t>
-  </si>
-  <si>
-    <t>How to Criticize - and Not Be Hated for It. 
-When you must criticize, try finding a way to do so indirectly. This is similar to the Poop Sandwich Method :  you have to be able to give hard news sometimes. When giving a Poop Sandwich, always use 'and' not 'but.' Most people begin their criticism with appreciation, but then follow it with the word "but" and go into the poopy news, such as "You've been working so hard and we really appreciate that, but..." Once someone hears the "but", it makes them question the sincerity of the appreciation. Try replacing the word "but" with "and". Example: "You've been working so hard and we really appreciate that, and we have some ideas on how to make all of your effort pay off even more. Here's what we were thinking..."</t>
-  </si>
-  <si>
-    <t>PrincipleType</t>
-  </si>
-  <si>
-    <t>Id</t>
+    <t>People naturally have their own agendas in the groups you lead.
+If you're too authoritarian they will resent you, and if you're too lax they will revert to doing their own interests.
+You need a chain of command where people buy into your vision and follow your lead naturally.
+The overall strategic vision must come from you and you alone. But make the group feel involved in the decision making. Take their good ideas, deflect the bad ones and if necessary make minor changes to appease the most political ones.
+The Dangers of Groupthink
+People in groups tend to act and speak conservatively as they're all worried of what others think.
+That's not what you need. And that's why you need unity of command (you).
+Beware of Political Animals
+Political animals not only are after themselves, but form factions to further their agendas and create their small fiefdoms of power.
+You should avoid hiring these people in the first place.
+Watch out for those who mirror your ideas 1:1, they're probably trying to ingratiate you.
+If it's too late, isolate them</t>
+  </si>
+  <si>
+    <t>Let them go first. Let them believe you're weak.
+Then destroy them with a counterattack once they're over-stretched.
+The best blows are the ones they never see coming</t>
+  </si>
+  <si>
+    <t>Sow the seeds of discontent, turn large enemies into smaller parts. Then attack and conquer.
+Romans divided the power base of their captured areas so that no one area had the power to attack.
+Divide groups and they are easier to conquer.
+Historically people have banded together to defend themselves, deny them this comfort.
+Surprise and splinter the group attacking the pieces.</t>
+  </si>
+  <si>
+    <t>Don't trust people's words.
+They will break their promises and find moral justifications for their amoral behaviors.
+And people will forget broken promises when you're strong and in the position to offer something they want.
+Keep advancing and waging wars during negotiations.
+When you keep winning the war you will get better deals and you can use the conquered terrain as bargaining chips. If on the other hand you stop, you will often find your enemy much stronger in battle because he didn't stop.
+It's even more important you keep advancing when you're holding the weak hand, so you can show resolve.
+Act strong and people will treat you as strong.</t>
+  </si>
+  <si>
+    <t>Most people operate with feelings and emotions and make alliances based on liking and friendships.
+Bad strategy: the best alliances are the ones giving something you can't get on your own.
+Sometimes we think instead that the more allies the better. But it's not true: the more you have, the more likely it is you'll be dragged into other people's wars.
+Alliances must be based on mutual interests. See them as stepping stones towards getting what you need.
+Finally, never become too dependent on alliances: they will drop you when it best serves them.
+Alliances Strategies:
+Seem like you want to help and let them do the work, then reap the benefits.
+You'll be accused of playing the alliance game, which are nothing but strategic moral attacks. The only real danger is that your reputation will be so tarnished that people won't want to ally with you anymore.
+But, says Greene:
+Self interest rules the world</t>
+  </si>
+  <si>
+    <t>Most people cling to status quo and loath of starting wars over trivial matters.
+That's why you will take small bites, bite by bite. Every time it will be too small to start a war and once you take enough bites they won't even be able to wage war against you.</t>
+  </si>
+  <si>
+    <t>Instead of fighting your enemies: join them.
+Infiltrate their ranks, rise to the top. Then slowly get what you want or stage a coup. Do not attack the walls of the fort, attack from within.
+Exploit the disaffected with your opponent and use them.
+Undermine the morale of your opponent's troops.
+Befriend your opponent and work from within their mind.
+Be patient and take small steps.
+Keep your group of conspirators small.</t>
+  </si>
+  <si>
+    <t>Terror strategies aim at raising havoc, making enemies fearful and provoking desperate overreactions -or surrenders without fighting.
+They serve well to smaller groups who can't fight openly because of size disparity.
+Their goal is to spread fear with small acts of violence that reverberate through stories and media and command outsized attention compared to their real effect.</t>
   </si>
 </sst>
 </file>
@@ -1305,11 +1303,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1626,14 +1627,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E06247-08F0-4AE8-93C2-6C2F86E254C8}">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E148"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="57.1796875" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
     <col min="3" max="3" width="115.36328125" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1647,10 +1649,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>302</v>
+        <v>212</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>303</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1658,13 +1660,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1675,13 +1677,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1692,13 +1694,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1709,13 +1711,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1726,13 +1728,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1743,13 +1745,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1760,13 +1762,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -1780,10 +1782,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -1800,41 +1802,41 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
+      <c r="C12" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E12">
         <v>11</v>
@@ -1845,13 +1847,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -1862,30 +1864,30 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E15">
         <v>14</v>
@@ -1896,13 +1898,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -1913,13 +1915,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -1930,47 +1932,47 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>256</v>
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>257</v>
+        <v>90</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E20">
         <v>19</v>
@@ -1981,64 +1983,64 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>258</v>
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>259</v>
+        <v>57</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>260</v>
+        <v>26</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>261</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E24">
         <v>23</v>
@@ -2049,98 +2051,98 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>297</v>
+        <v>28</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>263</v>
+        <v>59</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>264</v>
+        <v>196</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>298</v>
+        <v>29</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>266</v>
+        <v>205</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E30">
         <v>29</v>
@@ -2151,30 +2153,30 @@
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>267</v>
+        <v>206</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>299</v>
+        <v>31</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E32">
         <v>31</v>
@@ -2185,13 +2187,13 @@
         <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>268</v>
+        <v>207</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>300</v>
+        <v>211</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E33">
         <v>32</v>
@@ -2202,13 +2204,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>269</v>
+        <v>208</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E34">
         <v>33</v>
@@ -2219,13 +2221,13 @@
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>270</v>
+        <v>33</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E35">
         <v>34</v>
@@ -2236,30 +2238,30 @@
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>271</v>
+        <v>62</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>232</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E37">
         <v>36</v>
@@ -2270,30 +2272,30 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>272</v>
+        <v>209</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>273</v>
+        <v>35</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>268</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E39">
         <v>38</v>
@@ -2304,13 +2306,13 @@
         <v>21</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E40">
         <v>39</v>
@@ -2321,30 +2323,30 @@
         <v>22</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>23</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>301</v>
+        <v>39</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>269</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E42">
         <v>41</v>
@@ -2355,13 +2357,13 @@
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E43">
         <v>42</v>
@@ -2372,13 +2374,13 @@
         <v>25</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E44">
         <v>43</v>
@@ -2389,13 +2391,13 @@
         <v>26</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E45">
         <v>44</v>
@@ -2406,13 +2408,13 @@
         <v>27</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>69</v>
+        <v>44</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E46">
         <v>45</v>
@@ -2423,13 +2425,13 @@
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E47">
         <v>46</v>
@@ -2440,13 +2442,13 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E48">
         <v>47</v>
@@ -2457,13 +2459,13 @@
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="E49">
         <v>48</v>
@@ -2474,47 +2476,47 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>275</v>
+        <v>70</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>276</v>
+        <v>71</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E52">
         <v>51</v>
@@ -2525,13 +2527,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>277</v>
+        <v>72</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E53">
         <v>52</v>
@@ -2542,13 +2544,13 @@
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>278</v>
+        <v>73</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E54">
         <v>53</v>
@@ -2559,13 +2561,13 @@
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>279</v>
+        <v>74</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E55">
         <v>54</v>
@@ -2576,13 +2578,13 @@
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>280</v>
+        <v>75</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E56">
         <v>55</v>
@@ -2593,13 +2595,13 @@
         <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>281</v>
+        <v>76</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E57">
         <v>56</v>
@@ -2610,13 +2612,13 @@
         <v>9</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>282</v>
+        <v>77</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E58">
         <v>57</v>
@@ -2627,13 +2629,13 @@
         <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>283</v>
+        <v>78</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E59">
         <v>58</v>
@@ -2644,30 +2646,30 @@
         <v>11</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>284</v>
+        <v>79</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>12</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>205</v>
+        <v>80</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E61">
         <v>60</v>
@@ -2678,30 +2680,30 @@
         <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>285</v>
+        <v>83</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E63">
         <v>62</v>
@@ -2712,30 +2714,30 @@
         <v>15</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>286</v>
+        <v>84</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>16</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>287</v>
+        <v>85</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>281</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E65">
         <v>64</v>
@@ -2746,30 +2748,30 @@
         <v>17</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>18</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>288</v>
+        <v>88</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>282</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="E67">
         <v>66</v>
@@ -2780,64 +2782,64 @@
         <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>289</v>
+        <v>93</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>3</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>290</v>
+        <v>94</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>4</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>291</v>
+        <v>95</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>290</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E71">
         <v>70</v>
@@ -2848,13 +2850,13 @@
         <v>5</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E72">
         <v>71</v>
@@ -2865,13 +2867,13 @@
         <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E73">
         <v>72</v>
@@ -2882,13 +2884,13 @@
         <v>7</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>108</v>
+        <v>235</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E74">
         <v>73</v>
@@ -2899,13 +2901,13 @@
         <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>240</v>
+        <v>197</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E75">
         <v>74</v>
@@ -2916,13 +2918,13 @@
         <v>9</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>110</v>
+        <v>237</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E76">
         <v>75</v>
@@ -2933,13 +2935,13 @@
         <v>10</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>241</v>
+        <v>102</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E77">
         <v>76</v>
@@ -2950,13 +2952,13 @@
         <v>11</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>113</v>
+        <v>239</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E78">
         <v>77</v>
@@ -2967,13 +2969,13 @@
         <v>12</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E79">
         <v>78</v>
@@ -2984,13 +2986,13 @@
         <v>13</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>115</v>
+        <v>241</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E80">
         <v>79</v>
@@ -3001,13 +3003,13 @@
         <v>14</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E81">
         <v>80</v>
@@ -3018,13 +3020,13 @@
         <v>15</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>119</v>
+        <v>243</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E82">
         <v>81</v>
@@ -3035,13 +3037,13 @@
         <v>16</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E83">
         <v>82</v>
@@ -3052,13 +3054,13 @@
         <v>17</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>208</v>
+        <v>108</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>244</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E84">
         <v>83</v>
@@ -3069,13 +3071,13 @@
         <v>18</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E85">
         <v>84</v>
@@ -3086,13 +3088,13 @@
         <v>19</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>245</v>
+        <v>199</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E86">
         <v>85</v>
@@ -3103,13 +3105,13 @@
         <v>20</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E87">
         <v>86</v>
@@ -3120,13 +3122,13 @@
         <v>21</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>248</v>
+        <v>200</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E88">
         <v>87</v>
@@ -3137,13 +3139,13 @@
         <v>22</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E89">
         <v>88</v>
@@ -3154,13 +3156,13 @@
         <v>23</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E90">
         <v>89</v>
@@ -3171,13 +3173,13 @@
         <v>24</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E91">
         <v>90</v>
@@ -3188,13 +3190,13 @@
         <v>25</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>292</v>
+        <v>115</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E92">
         <v>91</v>
@@ -3205,13 +3207,13 @@
         <v>26</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E93">
         <v>92</v>
@@ -3222,13 +3224,13 @@
         <v>27</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>131</v>
+        <v>250</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E94">
         <v>93</v>
@@ -3239,13 +3241,13 @@
         <v>28</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E95">
         <v>94</v>
@@ -3256,13 +3258,13 @@
         <v>29</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E96">
         <v>95</v>
@@ -3273,30 +3275,30 @@
         <v>30</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>31</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>293</v>
+        <v>120</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E98">
         <v>97</v>
@@ -3307,13 +3309,13 @@
         <v>32</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>294</v>
+        <v>176</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E99">
         <v>98</v>
@@ -3324,13 +3326,13 @@
         <v>33</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E100">
         <v>99</v>
@@ -3341,13 +3343,13 @@
         <v>34</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>140</v>
+        <v>255</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E101">
         <v>100</v>
@@ -3358,13 +3360,13 @@
         <v>35</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E102">
         <v>101</v>
@@ -3375,13 +3377,13 @@
         <v>36</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>295</v>
+        <v>123</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E103">
         <v>102</v>
@@ -3392,13 +3394,13 @@
         <v>37</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E104">
         <v>103</v>
@@ -3409,13 +3411,13 @@
         <v>38</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>145</v>
+        <v>257</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E105">
         <v>104</v>
@@ -3426,13 +3428,13 @@
         <v>39</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>147</v>
+        <v>258</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E106">
         <v>105</v>
@@ -3443,13 +3445,13 @@
         <v>40</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>253</v>
+        <v>127</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E107">
         <v>106</v>
@@ -3460,13 +3462,13 @@
         <v>41</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>149</v>
+        <v>260</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E108">
         <v>107</v>
@@ -3477,13 +3479,13 @@
         <v>42</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E109">
         <v>108</v>
@@ -3494,13 +3496,13 @@
         <v>43</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E110">
         <v>109</v>
@@ -3511,13 +3513,13 @@
         <v>44</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>154</v>
+        <v>263</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E111">
         <v>110</v>
@@ -3528,13 +3530,13 @@
         <v>45</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>156</v>
+        <v>264</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E112">
         <v>111</v>
@@ -3545,13 +3547,13 @@
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>158</v>
+        <v>132</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E113">
         <v>112</v>
@@ -3562,13 +3564,13 @@
         <v>47</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>160</v>
+        <v>266</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E114">
         <v>113</v>
@@ -3579,30 +3581,30 @@
         <v>48</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>162</v>
+        <v>267</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E115">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>1</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>214</v>
+        <v>135</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E116">
         <v>115</v>
@@ -3613,13 +3615,13 @@
         <v>2</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E117">
         <v>116</v>
@@ -3630,47 +3632,47 @@
         <v>3</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E118">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>4</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>296</v>
+        <v>139</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E119">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>5</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>216</v>
+        <v>140</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E120">
         <v>119</v>
@@ -3681,30 +3683,30 @@
         <v>6</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>255</v>
+        <v>201</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E121">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>7</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C122" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="E122">
         <v>121</v>
@@ -3715,30 +3717,30 @@
         <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E123">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>9</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>219</v>
+        <v>144</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E124">
         <v>123</v>
@@ -3749,13 +3751,13 @@
         <v>10</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>220</v>
+        <v>182</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E125">
         <v>124</v>
@@ -3766,13 +3768,13 @@
         <v>11</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E126">
         <v>125</v>
@@ -3783,13 +3785,13 @@
         <v>12</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E127">
         <v>126</v>
@@ -3800,13 +3802,13 @@
         <v>13</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E128">
         <v>127</v>
@@ -3817,13 +3819,13 @@
         <v>14</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E129">
         <v>128</v>
@@ -3834,13 +3836,13 @@
         <v>15</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E130">
         <v>129</v>
@@ -3851,30 +3853,30 @@
         <v>16</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>224</v>
+        <v>186</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E131">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>17</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>184</v>
+        <v>154</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E132">
         <v>131</v>
@@ -3885,13 +3887,13 @@
         <v>18</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E133">
         <v>132</v>
@@ -3902,13 +3904,13 @@
         <v>19</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E134">
         <v>133</v>
@@ -3919,30 +3921,30 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E135">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>21</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>228</v>
+        <v>158</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E136">
         <v>135</v>
@@ -3953,13 +3955,13 @@
         <v>22</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E137">
         <v>136</v>
@@ -3970,13 +3972,13 @@
         <v>23</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>229</v>
+        <v>190</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E138">
         <v>137</v>
@@ -3987,13 +3989,13 @@
         <v>24</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E139">
         <v>138</v>
@@ -4004,13 +4006,13 @@
         <v>25</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E140">
         <v>139</v>
@@ -4021,30 +4023,30 @@
         <v>26</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E141">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>27</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>232</v>
+        <v>166</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>300</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E142">
         <v>141</v>
@@ -4055,30 +4057,30 @@
         <v>28</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>233</v>
+        <v>193</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E143">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>29</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>234</v>
+        <v>168</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>301</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E144">
         <v>143</v>
@@ -4089,30 +4091,30 @@
         <v>30</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E145">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>31</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>201</v>
+        <v>170</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>302</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E146">
         <v>145</v>
@@ -4123,30 +4125,30 @@
         <v>32</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E147">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>33</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>237</v>
+        <v>172</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E148">
         <v>147</v>

</xml_diff>

<commit_message>
- new random principle displayed every view of home page - button to show new random principle - allows linebreak of principle description
</commit_message>
<xml_diff>
--- a/InfluencePWA/Data/Source/influenceDataExcel.xlsx
+++ b/InfluencePWA/Data/Source/influenceDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hustler Joon\source\repos\InfluencePWA\InfluencePWA\Data\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CD1450-01B1-4545-9FA2-620D900E0AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3D6F02-FA55-48FD-88CD-FF7383EDC37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3705" windowWidth="29040" windowHeight="15840" xr2:uid="{3E2376BE-168A-49C5-9AFA-A2935957CF1D}"/>
   </bookViews>
@@ -44,10 +44,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Understand: the ability to connect deeply to your environment is the most primal and in many ways the most powerful form of mastery the brain can bring us. We gain such power by first transforming ourselves into consummate observers. We see everything in our surroundings as a potential sign to interpret. Nothing is taken at face value.
-To become such sensitive observers, we must not succumb to all of the distractions afforded by technology; we must be a little primitive. The primary instruments that we depend on must be our eyes for observing and our brains for analyzing.</t>
-  </si>
-  <si>
     <t>You must see whatever you produce as something that has a life and presence of its own. This presence can be vibrant and visceral, or it can be weak and lifeless.
 Seeing your work as something alive, your path to mastery is to study and absorb these details in a universal fashion, to the point at which you feel the life force and can express it effortlessly in your work.</t>
   </si>
@@ -761,33 +757,16 @@
 Break your forces into independent groups that can operate on their own. Give them the spirit of the campaign, a mission to accomplish, and room to run.</t>
   </si>
   <si>
-    <t>He Who Can Do This Has the Whole World with Him. 
-Before empathy became a buzzword, Carnegie was all about putting yourself in everyone else's shoes. The best metaphor in this chapter comes from David Lloyd George, former Prime Minister of the United Kingdom. He said he was able to maintain his power because he could "bait the hook to suit the fish." When you want to convince someone to buy your product, go into business with you, or agree with your idea, don't tell them why it will work, tell them why it will benefit them.
-Make Henry Ford's motto your own: "If there is any one secret to success, it lies in the ability to get the other person's point of view and see things from his angle as well as your own."</t>
-  </si>
-  <si>
     <t>Do This and You'll Be Welcome Anywhere. 
 Instead of thinking about how you can be impressive, aim to let others impress you. Invite them to tell you about their accomplishments and check in with them on both personal and professional endeavors. If you are comfortable, be the office cheerleader or a supporter of people in your network. Some ideas:
 Quote to post on your workspace: "We are interested in others when they are interested in us." - Publilius Syrus</t>
   </si>
   <si>
-    <t>If You Don't Do This, You Are Headed for Trouble. 
-We love hearing the sound of our own name. An easy way to make someone feel appreciated and heard is to show them you remember their name by using it regularly. This also means you have to work to remember names when you hear them. Create a system to remember people's names when you hear them. Or study up before meetings or networking events by looking over the RSVP list.
-Dale Carnegie summarizes this nicely: "The average person is more interested in his or her own name than in all the other names on Earth put together."</t>
-  </si>
-  <si>
-    <t>Never say, "You're wrong"</t>
-  </si>
-  <si>
     <t>If You're Wrong, Admit It. 
 Admitting you're wrong is actually a great way to build empathy, rapport and trust. Instead of avoiding your mistakes or trying to hide them, Carnegie encourages readers to admit wrongdoing "quickly, openly, and with enthusiasm." This helps people see you as human. And when you condemn yourself, other people seek to understand you and perhaps even defend you.</t>
   </si>
   <si>
     <t>Get the other person saying "yes, yes" as quickly as possible</t>
-  </si>
-  <si>
-    <t>The Safety Valve in Handling Complaints. 
-When people do not feel heard, understood or valued, they close up and shut down. If you are dealing with a difficult person, try finding the good in them. Remind them of their best day. La Rochefoucauld wisely said, "If you want enemies, excel your friends; but if you want friends, let your friends excel you."</t>
   </si>
   <si>
     <t>An Appeal That Everybody Likes. 
@@ -833,11 +812,6 @@
 The difference then is not in some initial creative power of the brain, but in how we look at the world and the fluidity with which we can reframe what we see. Creativity and adaptability are inseparable.</t>
   </si>
   <si>
-    <t>If You Want to Gather Honey, Don't Kick Over the Beehive. 
-Criticism more often is met with resentment than behavioral change. When you don't agree with someone, feel they have done wrong, or need to give someone negative feedback, it's hard not to be critical. However, Carnegie argues we cannot change behavior with threats or punishments. In his classic study, psychologist B.F. Skinner proved that when animals are rewarded for good behavior, they learn faster than animals punished for bad behavior.
-Let's follow Benjamin Franklin's wise advice: "I will speak ill of no man and speak all the good I know of everybody."</t>
-  </si>
-  <si>
     <t>An Easy Way to Become a Good Conversationalist. 
 We often think that being a good conversationalist means coming up with witty stories and funny jokes. But, actually, we like to hear ourselves talk. If you want to be seen as interesting, ask interesting questions and try to get the other person to open up. This doesn't mean you have to sit listening in silence. I like to think about listening as an active experience. Ask questions, use 'aha's' and 'wow's' and give them nonverbal encouragement.
 Are you really addicted to talking? Or worse, are you an interrupter? You might consider taking a Vow of Silence.</t>
@@ -847,11 +821,6 @@
 Treat other people in the way you yourself would like to be treated. Carnegie says that whenever you meet someone, you should ask yourself this basic question:
 "What is there about them that I can honestly admire?"
 Practice doing this with everyone you meet and pay special attention to people close to you.</t>
-  </si>
-  <si>
-    <t>You Can't Win an Argument. 
-Carnegie makes a great argument about arguing: you can't win. Even if you have the best possible stances and evidence, if you shoot down your opponent or make them feel wrong, they will resent you. So, even if you technically 'win,' you actually lose. This is especially hard in the age of data, instant Googling and research. If you want to prove someone wrong, see how you can discover what is right together.
-Abraham Lincoln wisely said, "No man who is resolved to make the most of himself can spare the time for personal contention."</t>
   </si>
   <si>
     <t>Speak through your work - be efficient, detail-oriented, and make what you write or present clear and easy to follow, and this will show your care for the audience or public at large.
@@ -870,41 +839,15 @@
 Advance through trial and error - learn as many skills as possible, but only related to your deepest interests. Find out what work suits you, and what doesn't. Be comfortable proceeding based on what you like, and when you are ready to settle, ideas and opportunities will present themselves to you.</t>
   </si>
   <si>
-    <t>The Big Secret of Dealing with People is making everyone feel important. 
-We don't do this with false flattery or brown nosing: there is nothing worse than an office suck-up. Carnegie argues the best way to make someone feel important is to be curious about them. When you are sitting with a colleague or chatting with someone at a networking event, ask questions that allow you to be sincerely interested.
-Follow Charles Schwab's lead, "I consider my ability to arouse enthusiasm among the men the greatest asset I possess, and the way to develop the best that is in a man is by appreciation and encouragement."</t>
-  </si>
-  <si>
     <t>A Simple Way to Make a Good First Impression. 
 Carnegie argues that a smile is the best way to show someone: "I like you. You make me happy. I am glad to see you."
 In a professional setting, a smile is not always needed. A warm greeting: yes! Acknowledgement of someone: definitely! Avoiding the negative: sure! But you do not have to walk around the office with a fake smile plastered to your face. It comes across as insincere and is not seen as professional.</t>
-  </si>
-  <si>
-    <t>How to Interest People. Look for people's hot buttons. 
-These are topics of conversations that light up people. You should know all of your colleagues hot buttons: what do they love to talk about? What do they spend their free time reading about? What gets them talking? Whenever you are with them, try to encourage them to talk about their most passionate interest and try to learn from them. This is the best way to get someone onto your side to show them you are interested in theirs.
-Listen to Teddy Roosevelt: "The royal road to a person's heart is to talk about the things he or she treasures most."</t>
   </si>
   <si>
     <t>A Sure Way of Making Enemies - and How to Avoid It.
 Every conflict or debate should start with a big dose of humility. We tend to think we are in the right all the time: immune to silly mistakes. However, if we go through life constantly thinking "I'm right," that makes others instantly wrong if they disagree with you. NO ONE likes to be wrong. Instead, be open to others' opinions. Carnegie's script for when you *think* someone is wrong. Say:
 "Well, now, look! I thought otherwise, but I may be wrong. I frequently am. And if I am wrong, I want to be put right. Let's examine the facts."
 Then proceed to discover the facts together.</t>
-  </si>
-  <si>
-    <t>The High Road to a Man's Reason is kindness. 
-No matter how angry, frustrated or upset you are: never start on a bad foot. There is almost no way to recover from a bad start. Woodrow Wilson put it best:
-"If you come at me with your fists doubled, I think I can promise you that mine will double as fast as yours; but if you come to me and say, 'Let us sit down and take counsel together, and, if we differ from one another, understand why it is that we differ from one another, just what the points at issue are,' we will presently find that we are not so far apart after all, that the points on which we differ are few and the points on which we agree are many, and that if we only have the patience and the candor and the desire to get together, we will get together."</t>
-  </si>
-  <si>
-    <t>How to Get Cooperation. 
-This is a hard one: but incredibly important. Carnegie argues that credit should not always be given where it is due. When you can, give up credit, offer praise, highlight someone's else's contribution.
-In the words of Lao Tzu:
-"The reason why rivers and seas receive the homage of a hundred mountain streams is that they keep below them. Thus they are able to reign over all the mountain streams. So the sage, wishing to be above men, putteth himself below them; wishing to be before them, he putteth himself behind them. Thus, though his place be above men, they do not feel his weight; though his place be before them, they do not count it an injury."</t>
-  </si>
-  <si>
-    <t>What Everybody Wants. Sympathy. 
-We all want to make sure that people understand our point of view. In fact, the more you can use someone else's words and tell them about their own opinions the better!
-Carnegie uses a magical phrase: "I don't blame you one iota for feeling as you do. If I were you, I should undoubtedly feel just as you do."</t>
   </si>
   <si>
     <t>If You Must Find Fault, This Is the Way to Begin. 
@@ -1242,6 +1185,63 @@
     <t>Terror strategies aim at raising havoc, making enemies fearful and provoking desperate overreactions -or surrenders without fighting.
 They serve well to smaller groups who can't fight openly because of size disparity.
 Their goal is to spread fear with small acts of violence that reverberate through stories and media and command outsized attention compared to their real effect.</t>
+  </si>
+  <si>
+    <t>Never say, "You're wrong"</t>
+  </si>
+  <si>
+    <t>How to Get Cooperation. 
+This is a hard one: but incredibly important. Carnegie argues that credit should not always be given where it is due. When you can, give up credit, offer praise, highlight someone's else's contribution.
+In the words of Lao Tzu:
+"The reason why rivers and seas receive the homage of a hundred mountain streams is that they keep below them. Thus they are able to reign over all the mountain streams. So the sage, wishing to be above men, putteth himself below them; wishing to be before them, he putteth himself behind them. Thus, though his place be above men, they do not feel his weight; though his place be before them, they do not count it an injury."</t>
+  </si>
+  <si>
+    <t>How to Interest People. Look for people's hot buttons. 
+These are topics of conversations that light up people. You should know all of your colleagues hot buttons: what do they love to talk about? What do they spend their free time reading about? What gets them talking? Whenever you are with them, try to encourage them to talk about their most passionate interest and try to learn from them. This is the best way to get someone onto your side to show them you are interested in theirs.
+Listen to Teddy Roosevelt: "The royal road to a person's heart is to talk about the things he or she treasures most."</t>
+  </si>
+  <si>
+    <t>If You Want to Gather Honey, Don't Kick Over the Beehive. 
+Criticism more often is met with resentment than behavioral change. When you don't agree with someone, feel they have done wrong, or need to give someone negative feedback, it's hard not to be critical. However, Carnegie argues we cannot change behavior with threats or punishments. In his classic study, psychologist B.F. Skinner proved that when animals are rewarded for good behavior, they learn faster than animals punished for bad behavior.
+Let's follow Benjamin Franklin's wise advice: "I will speak ill of no man and speak all the good I know of everybody."</t>
+  </si>
+  <si>
+    <t>The Big Secret of Dealing with People is making everyone feel important. 
+We don't do this with false flattery or brown nosing: there is nothing worse than an office suck-up. Carnegie argues the best way to make someone feel important is to be curious about them. When you are sitting with a colleague or chatting with someone at a networking event, ask questions that allow you to be sincerely interested.
+Follow Charles Schwab's lead, "I consider my ability to arouse enthusiasm among the men the greatest asset I possess, and the way to develop the best that is in a man is by appreciation and encouragement."</t>
+  </si>
+  <si>
+    <t>He Who Can Do This Has the Whole World with Him. 
+Before empathy became a buzzword, Carnegie was all about putting yourself in everyone else's shoes. The best metaphor in this chapter comes from David Lloyd George, former Prime Minister of the United Kingdom. He said he was able to maintain his power because he could "bait the hook to suit the fish." When you want to convince someone to buy your product, go into business with you, or agree with your idea, don't tell them why it will work, tell them why it will benefit them.
+Make Henry Ford's motto your own: "If there is any one secret to success, it lies in the ability to get the other person's point of view and see things from his angle as well as your own."</t>
+  </si>
+  <si>
+    <t>If You Don't Do This, You Are Headed for Trouble. 
+We love hearing the sound of our own name. An easy way to make someone feel appreciated and heard is to show them you remember their name by using it regularly. This also means you have to work to remember names when you hear them. Create a system to remember people's names when you hear them. Or study up before meetings or networking events by looking over the RSVP list.
+Dale Carnegie summarizes this nicely: "The average person is more interested in his or her own name than in all the other names on Earth put together."</t>
+  </si>
+  <si>
+    <t>You Can't Win an Argument. 
+Carnegie makes a great argument about arguing: you can't win. Even if you have the best possible stances and evidence, if you shoot down your opponent or make them feel wrong, they will resent you. So, even if you technically 'win,' you actually lose. This is especially hard in the age of data, instant Googling and research. If you want to prove someone wrong, see how you can discover what is right together.
+Abraham Lincoln wisely said, "No man who is resolved to make the most of himself can spare the time for personal contention."</t>
+  </si>
+  <si>
+    <t>The High Road to a Man's Reason is kindness. 
+No matter how angry, frustrated or upset you are: never start on a bad foot. There is almost no way to recover from a bad start. Woodrow Wilson put it best:
+"If you come at me with your fists doubled, I think I can promise you that mine will double as fast as yours; but if you come to me and say, 'Let us sit down and take counsel together, and, if we differ from one another, understand why it is that we differ from one another, just what the points at issue are,' we will presently find that we are not so far apart after all, that the points on which we differ are few and the points on which we agree are many, and that if we only have the patience and the candor and the desire to get together, we will get together."</t>
+  </si>
+  <si>
+    <t>The Safety Valve in Handling Complaints. 
+When people do not feel heard, understood or valued, they close up and shut down. If you are dealing with a difficult person, try finding the good in them. Remind them of their best day. La Rochefoucauld wisely said, "If you want enemies, excel your friends; but if you want friends, let your friends excel you."</t>
+  </si>
+  <si>
+    <t>What Everybody Wants. Sympathy. 
+We all want to make sure that people understand our point of view. In fact, the more you can use someone else's words and tell them about their own opinions the better!
+Carnegie uses a magical phrase: "I don't blame you one iota for feeling as you do. If I were you, I should undoubtedly feel just as you do."</t>
+  </si>
+  <si>
+    <t>Understand: the ability to connect deeply to your environment is the most primal and in many ways the most powerful form of mastery the brain can bring us. We gain such power by first transforming ourselves into consummate observers. We see everything in our surroundings as a potential sign to interpret. Nothing is taken at face value.
+To become such sensitive observers, we must not succumb to all of the distractions afforded by technology; we must be a little primitive. The primary instruments that we depend on must be our eyes for observing and our brains for analyzing.</t>
   </si>
 </sst>
 </file>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E06247-08F0-4AE8-93C2-6C2F86E254C8}">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1649,41 +1649,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1694,30 +1694,30 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1728,30 +1728,30 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -1762,47 +1762,47 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -1813,13 +1813,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1830,47 +1830,47 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14">
         <v>13</v>
@@ -1881,64 +1881,64 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1949,13 +1949,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19">
         <v>18</v>
@@ -1966,30 +1966,30 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E21">
         <v>20</v>
@@ -2000,13 +2000,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>202</v>
+        <v>297</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E22">
         <v>21</v>
@@ -2017,13 +2017,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E23">
         <v>22</v>
@@ -2034,30 +2034,30 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>204</v>
+        <v>57</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E25">
         <v>24</v>
@@ -2068,13 +2068,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E26">
         <v>25</v>
@@ -2085,13 +2085,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>228</v>
+        <v>294</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E27">
         <v>26</v>
@@ -2102,13 +2102,13 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E28">
         <v>27</v>
@@ -2119,13 +2119,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>223</v>
+        <v>299</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E29">
         <v>28</v>
@@ -2136,30 +2136,30 @@
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>205</v>
+        <v>292</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>206</v>
+        <v>29</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -2170,81 +2170,81 @@
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>208</v>
+        <v>31</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>301</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>231</v>
+        <v>293</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E36">
         <v>35</v>
@@ -2255,30 +2255,30 @@
         <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>232</v>
+        <v>302</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="E38">
         <v>37</v>
@@ -2289,47 +2289,47 @@
         <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>21</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>22</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E41">
         <v>40</v>
@@ -2340,149 +2340,149 @@
         <v>23</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>24</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>25</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>26</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>27</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>210</v>
+        <v>64</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="D50" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E50">
         <v>49</v>
@@ -2493,13 +2493,13 @@
         <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E51">
         <v>50</v>
@@ -2510,149 +2510,149 @@
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>9</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>10</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>11</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E60">
         <v>59</v>
@@ -2663,30 +2663,30 @@
         <v>12</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D62" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E62">
         <v>61</v>
@@ -2697,30 +2697,30 @@
         <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>15</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E64">
         <v>63</v>
@@ -2731,13 +2731,13 @@
         <v>16</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E65">
         <v>64</v>
@@ -2748,13 +2748,13 @@
         <v>17</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="D66" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E66">
         <v>65</v>
@@ -2765,13 +2765,13 @@
         <v>18</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E67">
         <v>66</v>
@@ -2782,13 +2782,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D68" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E68">
         <v>67</v>
@@ -2799,13 +2799,13 @@
         <v>2</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E69">
         <v>68</v>
@@ -2816,13 +2816,13 @@
         <v>3</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E70">
         <v>69</v>
@@ -2833,13 +2833,13 @@
         <v>4</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E71">
         <v>70</v>
@@ -2850,13 +2850,13 @@
         <v>5</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D72" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E72">
         <v>71</v>
@@ -2867,13 +2867,13 @@
         <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D73" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E73">
         <v>72</v>
@@ -2884,30 +2884,30 @@
         <v>7</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>8</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E75">
         <v>74</v>
@@ -2918,30 +2918,30 @@
         <v>9</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>10</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E77">
         <v>76</v>
@@ -2952,13 +2952,13 @@
         <v>11</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E78">
         <v>77</v>
@@ -2969,13 +2969,13 @@
         <v>12</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E79">
         <v>78</v>
@@ -2986,13 +2986,13 @@
         <v>13</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E80">
         <v>79</v>
@@ -3003,13 +3003,13 @@
         <v>14</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E81">
         <v>80</v>
@@ -3020,13 +3020,13 @@
         <v>15</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E82">
         <v>81</v>
@@ -3037,30 +3037,30 @@
         <v>16</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>17</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E84">
         <v>83</v>
@@ -3071,13 +3071,13 @@
         <v>18</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E85">
         <v>84</v>
@@ -3088,13 +3088,13 @@
         <v>19</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E86">
         <v>85</v>
@@ -3105,30 +3105,30 @@
         <v>20</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="D87" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>21</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E88">
         <v>87</v>
@@ -3139,13 +3139,13 @@
         <v>22</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="D89" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E89">
         <v>88</v>
@@ -3156,13 +3156,13 @@
         <v>23</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E90">
         <v>89</v>
@@ -3173,30 +3173,30 @@
         <v>24</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>25</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E92">
         <v>91</v>
@@ -3207,13 +3207,13 @@
         <v>26</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E93">
         <v>92</v>
@@ -3224,30 +3224,30 @@
         <v>27</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>28</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E95">
         <v>94</v>
@@ -3258,13 +3258,13 @@
         <v>29</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E96">
         <v>95</v>
@@ -3275,13 +3275,13 @@
         <v>30</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E97">
         <v>96</v>
@@ -3292,30 +3292,30 @@
         <v>31</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>32</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E99">
         <v>98</v>
@@ -3326,13 +3326,13 @@
         <v>33</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E100">
         <v>99</v>
@@ -3343,13 +3343,13 @@
         <v>34</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E101">
         <v>100</v>
@@ -3360,30 +3360,30 @@
         <v>35</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E102">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>36</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E103">
         <v>102</v>
@@ -3394,13 +3394,13 @@
         <v>37</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E104">
         <v>103</v>
@@ -3411,13 +3411,13 @@
         <v>38</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E105">
         <v>104</v>
@@ -3428,30 +3428,30 @@
         <v>39</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E106">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>40</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E107">
         <v>106</v>
@@ -3462,13 +3462,13 @@
         <v>41</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E108">
         <v>107</v>
@@ -3479,13 +3479,13 @@
         <v>42</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E109">
         <v>108</v>
@@ -3496,13 +3496,13 @@
         <v>43</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E110">
         <v>109</v>
@@ -3513,13 +3513,13 @@
         <v>44</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E111">
         <v>110</v>
@@ -3530,30 +3530,30 @@
         <v>45</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E112">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E113">
         <v>112</v>
@@ -3564,13 +3564,13 @@
         <v>47</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E114">
         <v>113</v>
@@ -3581,13 +3581,13 @@
         <v>48</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E115">
         <v>114</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E116">
         <v>115</v>
@@ -3615,13 +3615,13 @@
         <v>2</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E117">
         <v>116</v>
@@ -3632,13 +3632,13 @@
         <v>3</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E118">
         <v>117</v>
@@ -3649,13 +3649,13 @@
         <v>4</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E119">
         <v>118</v>
@@ -3666,13 +3666,13 @@
         <v>5</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E120">
         <v>119</v>
@@ -3683,13 +3683,13 @@
         <v>6</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E121">
         <v>120</v>
@@ -3700,13 +3700,13 @@
         <v>7</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E122">
         <v>121</v>
@@ -3717,13 +3717,13 @@
         <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E123">
         <v>122</v>
@@ -3734,13 +3734,13 @@
         <v>9</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E124">
         <v>123</v>
@@ -3751,13 +3751,13 @@
         <v>10</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E125">
         <v>124</v>
@@ -3768,13 +3768,13 @@
         <v>11</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E126">
         <v>125</v>
@@ -3785,13 +3785,13 @@
         <v>12</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="D127" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E127">
         <v>126</v>
@@ -3802,13 +3802,13 @@
         <v>13</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E128">
         <v>127</v>
@@ -3819,13 +3819,13 @@
         <v>14</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="D129" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E129">
         <v>128</v>
@@ -3836,13 +3836,13 @@
         <v>15</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E130">
         <v>129</v>
@@ -3853,13 +3853,13 @@
         <v>16</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E131">
         <v>130</v>
@@ -3870,13 +3870,13 @@
         <v>17</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E132">
         <v>131</v>
@@ -3887,13 +3887,13 @@
         <v>18</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E133">
         <v>132</v>
@@ -3904,13 +3904,13 @@
         <v>19</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E134">
         <v>133</v>
@@ -3921,13 +3921,13 @@
         <v>20</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E135">
         <v>134</v>
@@ -3938,13 +3938,13 @@
         <v>21</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E136">
         <v>135</v>
@@ -3955,13 +3955,13 @@
         <v>22</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="D137" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E137">
         <v>136</v>
@@ -3972,13 +3972,13 @@
         <v>23</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E138">
         <v>137</v>
@@ -3989,13 +3989,13 @@
         <v>24</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E139">
         <v>138</v>
@@ -4006,13 +4006,13 @@
         <v>25</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E140">
         <v>139</v>
@@ -4023,13 +4023,13 @@
         <v>26</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="D141" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E141">
         <v>140</v>
@@ -4040,13 +4040,13 @@
         <v>27</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E142">
         <v>141</v>
@@ -4057,13 +4057,13 @@
         <v>28</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E143">
         <v>142</v>
@@ -4074,13 +4074,13 @@
         <v>29</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E144">
         <v>143</v>
@@ -4091,13 +4091,13 @@
         <v>30</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E145">
         <v>144</v>
@@ -4108,13 +4108,13 @@
         <v>31</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E146">
         <v>145</v>
@@ -4125,13 +4125,13 @@
         <v>32</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E147">
         <v>146</v>
@@ -4142,13 +4142,13 @@
         <v>33</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E148">
         <v>147</v>

</xml_diff>